<commit_message>
Colocando uns detalhes q esqueci na planilha de testes...
</commit_message>
<xml_diff>
--- a/War/Testes/Casos de Teste/Casos de Teste.xlsx
+++ b/War/Testes/Casos de Teste/Casos de Teste.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Teste" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="299">
   <si>
     <t>Nome do Caso de Teste:</t>
   </si>
@@ -920,6 +920,9 @@
   </si>
   <si>
     <t>15.1 até 15.3</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -1245,9 +1248,50 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1259,30 +1303,13 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="11" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="12" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1294,21 +1321,7 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="11" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="12" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="Bom 2" xfId="2"/>
@@ -1632,46 +1645,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A246" workbookViewId="0">
-      <selection activeCell="B303" sqref="B303:E303"/>
+    <sheetView topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2" style="8" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.7109375" style="18" customWidth="1"/>
-    <col min="4" max="5" width="23.7109375" style="18" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="2" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" style="10" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="17">
         <v>1</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -1687,53 +1701,53 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="9">
+    <row r="6" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
         <v>1</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="8" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="16"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="17">
         <v>2</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="4"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="4"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -1749,65 +1763,65 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B13" s="9">
+    <row r="13" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
         <v>1</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="7" t="s">
         <v>43</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="14" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B14" s="9">
+    <row r="14" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
         <v>2</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="7" t="s">
         <v>36</v>
       </c>
       <c r="E14" s="21"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="16"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="17">
         <v>3</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="4"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="19"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="4"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="19"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="14"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="13"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
@@ -1823,65 +1837,65 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B21" s="9">
+    <row r="21" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B21" s="3">
         <v>1</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="7" t="s">
         <v>43</v>
       </c>
       <c r="E21" s="20" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="22" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B22" s="9">
+    <row r="22" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B22" s="3">
         <v>2</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="7" t="s">
         <v>38</v>
       </c>
       <c r="E22" s="21"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="16"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="17">
         <v>4</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="4"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="19"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="4"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="19"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="14"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="13"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
@@ -1897,77 +1911,77 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B29" s="9">
+    <row r="29" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B29" s="3">
         <v>1</v>
       </c>
-      <c r="C29" s="19" t="s">
+      <c r="C29" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D29" s="7" t="s">
         <v>43</v>
       </c>
       <c r="E29" s="20" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="30" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B30" s="9">
+    <row r="30" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B30" s="3">
         <v>2</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="C30" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D30" s="19" t="s">
+      <c r="D30" s="7" t="s">
         <v>38</v>
       </c>
       <c r="E30" s="22"/>
     </row>
-    <row r="31" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B31" s="9">
+    <row r="31" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B31" s="3">
         <v>3</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C31" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="7" t="s">
         <v>40</v>
       </c>
       <c r="E31" s="21"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="5"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="7"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="16"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="17">
         <v>5</v>
       </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="4"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="19"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="4"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="19"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="14"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="13"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
@@ -1983,53 +1997,53 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B38" s="9">
+    <row r="38" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B38" s="3">
         <v>1</v>
       </c>
-      <c r="C38" s="19" t="s">
+      <c r="C38" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E38" s="19" t="s">
+      <c r="E38" s="8" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="5"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="7"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="16"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="17">
         <v>6</v>
       </c>
-      <c r="D41" s="3"/>
-      <c r="E41" s="4"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="19"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="4"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="19"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="12"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="14"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="13"/>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
@@ -2045,65 +2059,65 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B45" s="9">
+    <row r="45" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B45" s="3">
         <v>1</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="C45" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D45" s="19" t="s">
+      <c r="D45" s="7" t="s">
         <v>42</v>
       </c>
       <c r="E45" s="20" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="46" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B46" s="9">
+    <row r="46" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B46" s="3">
         <v>2</v>
       </c>
-      <c r="C46" s="19" t="s">
+      <c r="C46" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D46" s="19" t="s">
+      <c r="D46" s="7" t="s">
         <v>36</v>
       </c>
       <c r="E46" s="21"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="5"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="7"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="16"/>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="17">
         <v>7</v>
       </c>
-      <c r="D49" s="3"/>
-      <c r="E49" s="4"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="19"/>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D50" s="3"/>
-      <c r="E50" s="4"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="19"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C51" s="12"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="14"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="13"/>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
@@ -2119,53 +2133,53 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B53" s="9">
+    <row r="53" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B53" s="3">
         <v>1</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="C53" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D53" s="19" t="s">
+      <c r="D53" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E53" s="19" t="s">
+      <c r="E53" s="8" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="5"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="7"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="16"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="17">
         <v>8</v>
       </c>
-      <c r="D56" s="3"/>
-      <c r="E56" s="4"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="19"/>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D57" s="3"/>
-      <c r="E57" s="4"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="19"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C58" s="12"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="14"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="13"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
@@ -2181,77 +2195,77 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B60" s="9">
+    <row r="60" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B60" s="3">
         <v>1</v>
       </c>
-      <c r="C60" s="19" t="s">
+      <c r="C60" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D60" s="19" t="s">
+      <c r="D60" s="7" t="s">
         <v>46</v>
       </c>
       <c r="E60" s="20" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="61" spans="2:5" s="11" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B61" s="9">
+    <row r="61" spans="2:5" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B61" s="3">
         <v>2</v>
       </c>
-      <c r="C61" s="19" t="s">
+      <c r="C61" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="D61" s="19" t="s">
+      <c r="D61" s="7" t="s">
         <v>49</v>
       </c>
       <c r="E61" s="22"/>
     </row>
-    <row r="62" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B62" s="9">
+    <row r="62" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B62" s="3">
         <v>3</v>
       </c>
-      <c r="C62" s="19" t="s">
+      <c r="C62" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D62" s="19" t="s">
+      <c r="D62" s="7" t="s">
         <v>48</v>
       </c>
       <c r="E62" s="21"/>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="5"/>
-      <c r="C63" s="6"/>
-      <c r="D63" s="6"/>
-      <c r="E63" s="7"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="16"/>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C65" s="17">
         <v>9</v>
       </c>
-      <c r="D65" s="3"/>
-      <c r="E65" s="4"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="19"/>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C66" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D66" s="3"/>
-      <c r="E66" s="4"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="19"/>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C67" s="12"/>
-      <c r="D67" s="13"/>
-      <c r="E67" s="14"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="13"/>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
@@ -2267,77 +2281,77 @@
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B69" s="9">
+    <row r="69" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B69" s="3">
         <v>1</v>
       </c>
-      <c r="C69" s="19" t="s">
+      <c r="C69" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D69" s="19" t="s">
+      <c r="D69" s="7" t="s">
         <v>46</v>
       </c>
       <c r="E69" s="20" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="70" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B70" s="9">
+    <row r="70" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B70" s="3">
         <v>2</v>
       </c>
-      <c r="C70" s="19" t="s">
+      <c r="C70" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="D70" s="19" t="s">
+      <c r="D70" s="7" t="s">
         <v>49</v>
       </c>
       <c r="E70" s="22"/>
     </row>
-    <row r="71" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="9">
+    <row r="71" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="3">
         <v>3</v>
       </c>
-      <c r="C71" s="19" t="s">
+      <c r="C71" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D71" s="19" t="s">
+      <c r="D71" s="7" t="s">
         <v>149</v>
       </c>
       <c r="E71" s="21"/>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B72" s="5"/>
-      <c r="C72" s="6"/>
-      <c r="D72" s="6"/>
-      <c r="E72" s="7"/>
+      <c r="B72" s="14"/>
+      <c r="C72" s="15"/>
+      <c r="D72" s="15"/>
+      <c r="E72" s="16"/>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C74" s="2">
+      <c r="C74" s="17">
         <v>10</v>
       </c>
-      <c r="D74" s="3"/>
-      <c r="E74" s="4"/>
+      <c r="D74" s="18"/>
+      <c r="E74" s="19"/>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C75" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D75" s="3"/>
-      <c r="E75" s="4"/>
+      <c r="D75" s="18"/>
+      <c r="E75" s="19"/>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C76" s="12"/>
-      <c r="D76" s="13"/>
-      <c r="E76" s="14"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="13"/>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
@@ -2353,67 +2367,67 @@
         <v>30</v>
       </c>
     </row>
-    <row r="78" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B78" s="9">
+    <row r="78" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B78" s="3">
         <v>1</v>
       </c>
-      <c r="C78" s="19" t="s">
+      <c r="C78" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D78" s="19" t="s">
+      <c r="D78" s="7" t="s">
         <v>46</v>
       </c>
       <c r="E78" s="20" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="79" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B79" s="9">
+    <row r="79" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B79" s="3">
         <v>2</v>
       </c>
-      <c r="C79" s="19" t="s">
+      <c r="C79" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D79" s="19" t="s">
+      <c r="D79" s="7" t="s">
         <v>36</v>
       </c>
       <c r="E79" s="21"/>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B80" s="5"/>
-      <c r="C80" s="6"/>
-      <c r="D80" s="6"/>
-      <c r="E80" s="7"/>
+      <c r="B80" s="14"/>
+      <c r="C80" s="15"/>
+      <c r="D80" s="15"/>
+      <c r="E80" s="16"/>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C82" s="2">
+      <c r="C82" s="17">
         <v>11</v>
       </c>
-      <c r="D82" s="3"/>
-      <c r="E82" s="4"/>
+      <c r="D82" s="18"/>
+      <c r="E82" s="19"/>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C83" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D83" s="3"/>
-      <c r="E83" s="4"/>
+      <c r="D83" s="18"/>
+      <c r="E83" s="19"/>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C84" s="15" t="s">
+      <c r="C84" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D84" s="16"/>
-      <c r="E84" s="17"/>
+      <c r="D84" s="24"/>
+      <c r="E84" s="25"/>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85" s="1" t="s">
@@ -2429,53 +2443,53 @@
         <v>30</v>
       </c>
     </row>
-    <row r="86" spans="2:5" s="11" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="B86" s="9"/>
-      <c r="C86" s="19" t="s">
+    <row r="86" spans="2:5" s="5" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="B86" s="3"/>
+      <c r="C86" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D86" s="19" t="s">
+      <c r="D86" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E86" s="19" t="s">
+      <c r="E86" s="8" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B87" s="5"/>
-      <c r="C87" s="6"/>
-      <c r="D87" s="6"/>
-      <c r="E87" s="7"/>
+      <c r="B87" s="14"/>
+      <c r="C87" s="15"/>
+      <c r="D87" s="15"/>
+      <c r="E87" s="16"/>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C89" s="2">
+      <c r="C89" s="17">
         <v>12</v>
       </c>
-      <c r="D89" s="3"/>
-      <c r="E89" s="4"/>
+      <c r="D89" s="18"/>
+      <c r="E89" s="19"/>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C90" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D90" s="3"/>
-      <c r="E90" s="4"/>
+      <c r="D90" s="18"/>
+      <c r="E90" s="19"/>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B91" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C91" s="15" t="s">
+      <c r="C91" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D91" s="16"/>
-      <c r="E91" s="17"/>
+      <c r="D91" s="24"/>
+      <c r="E91" s="25"/>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" s="1" t="s">
@@ -2491,55 +2505,55 @@
         <v>30</v>
       </c>
     </row>
-    <row r="93" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B93" s="9">
+    <row r="93" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B93" s="3">
         <v>1</v>
       </c>
-      <c r="C93" s="19" t="s">
+      <c r="C93" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D93" s="19" t="s">
+      <c r="D93" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E93" s="19" t="s">
+      <c r="E93" s="8" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B94" s="5"/>
-      <c r="C94" s="6"/>
-      <c r="D94" s="6"/>
-      <c r="E94" s="7"/>
+      <c r="B94" s="14"/>
+      <c r="C94" s="15"/>
+      <c r="D94" s="15"/>
+      <c r="E94" s="16"/>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C96" s="2">
+      <c r="C96" s="17">
         <v>13</v>
       </c>
-      <c r="D96" s="3"/>
-      <c r="E96" s="4"/>
+      <c r="D96" s="18"/>
+      <c r="E96" s="19"/>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="C97" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D97" s="3"/>
-      <c r="E97" s="4"/>
+      <c r="D97" s="18"/>
+      <c r="E97" s="19"/>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B98" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C98" s="15" t="s">
+      <c r="C98" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D98" s="16"/>
-      <c r="E98" s="17"/>
+      <c r="D98" s="24"/>
+      <c r="E98" s="25"/>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B99" s="1" t="s">
@@ -2555,67 +2569,67 @@
         <v>30</v>
       </c>
     </row>
-    <row r="100" spans="2:5" s="11" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="B100" s="9">
+    <row r="100" spans="2:5" s="5" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="B100" s="3">
         <v>1</v>
       </c>
-      <c r="C100" s="19" t="s">
+      <c r="C100" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D100" s="19" t="s">
+      <c r="D100" s="7" t="s">
         <v>55</v>
       </c>
       <c r="E100" s="20" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="101" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B101" s="9">
+    <row r="101" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B101" s="3">
         <v>2</v>
       </c>
-      <c r="C101" s="19" t="s">
+      <c r="C101" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D101" s="19" t="s">
+      <c r="D101" s="7" t="s">
         <v>58</v>
       </c>
       <c r="E101" s="21"/>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B102" s="5"/>
-      <c r="C102" s="6"/>
-      <c r="D102" s="6"/>
-      <c r="E102" s="7"/>
+      <c r="B102" s="14"/>
+      <c r="C102" s="15"/>
+      <c r="D102" s="15"/>
+      <c r="E102" s="16"/>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B104" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C104" s="2">
+      <c r="C104" s="17">
         <v>14</v>
       </c>
-      <c r="D104" s="3"/>
-      <c r="E104" s="4"/>
+      <c r="D104" s="18"/>
+      <c r="E104" s="19"/>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B105" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C105" s="2" t="s">
+      <c r="C105" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="D105" s="3"/>
-      <c r="E105" s="4"/>
+      <c r="D105" s="18"/>
+      <c r="E105" s="19"/>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B106" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C106" s="15" t="s">
+      <c r="C106" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D106" s="16"/>
-      <c r="E106" s="17"/>
+      <c r="D106" s="24"/>
+      <c r="E106" s="25"/>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B107" s="1" t="s">
@@ -2631,67 +2645,67 @@
         <v>30</v>
       </c>
     </row>
-    <row r="108" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B108" s="9">
+    <row r="108" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B108" s="3">
         <v>1</v>
       </c>
-      <c r="C108" s="19" t="s">
+      <c r="C108" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D108" s="19" t="s">
+      <c r="D108" s="7" t="s">
         <v>57</v>
       </c>
       <c r="E108" s="20" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="109" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B109" s="9">
+    <row r="109" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B109" s="3">
         <v>2</v>
       </c>
-      <c r="C109" s="19" t="s">
+      <c r="C109" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D109" s="19" t="s">
+      <c r="D109" s="7" t="s">
         <v>68</v>
       </c>
       <c r="E109" s="21"/>
     </row>
     <row r="110" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B110" s="5"/>
-      <c r="C110" s="6"/>
-      <c r="D110" s="6"/>
-      <c r="E110" s="7"/>
+      <c r="B110" s="14"/>
+      <c r="C110" s="15"/>
+      <c r="D110" s="15"/>
+      <c r="E110" s="16"/>
     </row>
     <row r="112" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B112" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C112" s="2">
+      <c r="C112" s="17">
         <v>15</v>
       </c>
-      <c r="D112" s="3"/>
-      <c r="E112" s="4"/>
+      <c r="D112" s="18"/>
+      <c r="E112" s="19"/>
     </row>
     <row r="113" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B113" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C113" s="2" t="s">
+      <c r="C113" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D113" s="3"/>
-      <c r="E113" s="4"/>
+      <c r="D113" s="18"/>
+      <c r="E113" s="19"/>
     </row>
     <row r="114" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C114" s="15" t="s">
+      <c r="C114" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="D114" s="16"/>
-      <c r="E114" s="17"/>
+      <c r="D114" s="24"/>
+      <c r="E114" s="25"/>
     </row>
     <row r="115" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B115" s="1" t="s">
@@ -2707,79 +2721,79 @@
         <v>30</v>
       </c>
     </row>
-    <row r="116" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B116" s="9">
+    <row r="116" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B116" s="3">
         <v>1</v>
       </c>
-      <c r="C116" s="19" t="s">
+      <c r="C116" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D116" s="19" t="s">
+      <c r="D116" s="7" t="s">
         <v>57</v>
       </c>
       <c r="E116" s="20" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="117" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B117" s="9">
+    <row r="117" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B117" s="3">
         <v>2</v>
       </c>
-      <c r="C117" s="19" t="s">
+      <c r="C117" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D117" s="19" t="s">
+      <c r="D117" s="7" t="s">
         <v>60</v>
       </c>
       <c r="E117" s="22"/>
     </row>
-    <row r="118" spans="2:5" s="11" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="B118" s="9">
+    <row r="118" spans="2:5" s="5" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="B118" s="3">
         <v>3</v>
       </c>
-      <c r="C118" s="19" t="s">
+      <c r="C118" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D118" s="19" t="s">
+      <c r="D118" s="7" t="s">
         <v>63</v>
       </c>
       <c r="E118" s="21"/>
     </row>
     <row r="119" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B119" s="5"/>
-      <c r="C119" s="6"/>
-      <c r="D119" s="6"/>
-      <c r="E119" s="7"/>
+      <c r="B119" s="14"/>
+      <c r="C119" s="15"/>
+      <c r="D119" s="15"/>
+      <c r="E119" s="16"/>
     </row>
     <row r="121" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B121" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C121" s="2">
+      <c r="C121" s="17">
         <v>16</v>
       </c>
-      <c r="D121" s="3"/>
-      <c r="E121" s="4"/>
+      <c r="D121" s="18"/>
+      <c r="E121" s="19"/>
     </row>
     <row r="122" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B122" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="C122" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D122" s="3"/>
-      <c r="E122" s="4"/>
+      <c r="D122" s="18"/>
+      <c r="E122" s="19"/>
     </row>
     <row r="123" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B123" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C123" s="15" t="s">
+      <c r="C123" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D123" s="16"/>
-      <c r="E123" s="17"/>
+      <c r="D123" s="24"/>
+      <c r="E123" s="25"/>
     </row>
     <row r="124" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B124" s="1" t="s">
@@ -2795,67 +2809,67 @@
         <v>30</v>
       </c>
     </row>
-    <row r="125" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B125" s="9">
+    <row r="125" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B125" s="3">
         <v>1</v>
       </c>
-      <c r="C125" s="19" t="s">
+      <c r="C125" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D125" s="19" t="s">
+      <c r="D125" s="7" t="s">
         <v>57</v>
       </c>
       <c r="E125" s="20" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="126" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B126" s="9">
+    <row r="126" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B126" s="3">
         <v>2</v>
       </c>
-      <c r="C126" s="19" t="s">
+      <c r="C126" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D126" s="19" t="s">
+      <c r="D126" s="7" t="s">
         <v>65</v>
       </c>
       <c r="E126" s="21"/>
     </row>
     <row r="127" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B127" s="5"/>
-      <c r="C127" s="6"/>
-      <c r="D127" s="6"/>
-      <c r="E127" s="7"/>
+      <c r="B127" s="14"/>
+      <c r="C127" s="15"/>
+      <c r="D127" s="15"/>
+      <c r="E127" s="16"/>
     </row>
     <row r="129" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B129" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C129" s="2">
+      <c r="C129" s="17">
         <v>17</v>
       </c>
-      <c r="D129" s="3"/>
-      <c r="E129" s="4"/>
+      <c r="D129" s="18"/>
+      <c r="E129" s="19"/>
     </row>
     <row r="130" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B130" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C130" s="2" t="s">
+      <c r="C130" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D130" s="3"/>
-      <c r="E130" s="4"/>
+      <c r="D130" s="18"/>
+      <c r="E130" s="19"/>
     </row>
     <row r="131" spans="2:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B131" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C131" s="15" t="s">
+      <c r="C131" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D131" s="16"/>
-      <c r="E131" s="17"/>
+      <c r="D131" s="24"/>
+      <c r="E131" s="25"/>
     </row>
     <row r="132" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B132" s="1" t="s">
@@ -2871,67 +2885,67 @@
         <v>30</v>
       </c>
     </row>
-    <row r="133" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B133" s="9">
+    <row r="133" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B133" s="3">
         <v>1</v>
       </c>
-      <c r="C133" s="19" t="s">
+      <c r="C133" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D133" s="19" t="s">
+      <c r="D133" s="7" t="s">
         <v>73</v>
       </c>
       <c r="E133" s="20" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="134" spans="2:5" s="11" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B134" s="9">
+    <row r="134" spans="2:5" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B134" s="3">
         <v>2</v>
       </c>
-      <c r="C134" s="19" t="s">
+      <c r="C134" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D134" s="19" t="s">
+      <c r="D134" s="7" t="s">
         <v>71</v>
       </c>
       <c r="E134" s="21"/>
     </row>
     <row r="135" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B135" s="5"/>
-      <c r="C135" s="6"/>
-      <c r="D135" s="6"/>
-      <c r="E135" s="7"/>
+      <c r="B135" s="14"/>
+      <c r="C135" s="15"/>
+      <c r="D135" s="15"/>
+      <c r="E135" s="16"/>
     </row>
     <row r="137" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B137" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C137" s="2">
+      <c r="C137" s="17">
         <v>18</v>
       </c>
-      <c r="D137" s="3"/>
-      <c r="E137" s="4"/>
+      <c r="D137" s="18"/>
+      <c r="E137" s="19"/>
     </row>
     <row r="138" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B138" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C138" s="2" t="s">
+      <c r="C138" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D138" s="3"/>
-      <c r="E138" s="4"/>
+      <c r="D138" s="18"/>
+      <c r="E138" s="19"/>
     </row>
     <row r="139" spans="2:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B139" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C139" s="15" t="s">
+      <c r="C139" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D139" s="16"/>
-      <c r="E139" s="17"/>
+      <c r="D139" s="24"/>
+      <c r="E139" s="25"/>
     </row>
     <row r="140" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B140" s="1" t="s">
@@ -2947,55 +2961,55 @@
         <v>30</v>
       </c>
     </row>
-    <row r="141" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B141" s="9">
+    <row r="141" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B141" s="3">
         <v>1</v>
       </c>
-      <c r="C141" s="19" t="s">
+      <c r="C141" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D141" s="19" t="s">
+      <c r="D141" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="E141" s="19" t="s">
+      <c r="E141" s="8" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="142" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B142" s="5"/>
-      <c r="C142" s="6"/>
-      <c r="D142" s="6"/>
-      <c r="E142" s="7"/>
+      <c r="B142" s="14"/>
+      <c r="C142" s="15"/>
+      <c r="D142" s="15"/>
+      <c r="E142" s="16"/>
     </row>
     <row r="144" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B144" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C144" s="2">
+      <c r="C144" s="17">
         <v>19</v>
       </c>
-      <c r="D144" s="3"/>
-      <c r="E144" s="4"/>
+      <c r="D144" s="18"/>
+      <c r="E144" s="19"/>
     </row>
     <row r="145" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B145" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C145" s="2" t="s">
+      <c r="C145" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D145" s="3"/>
-      <c r="E145" s="4"/>
+      <c r="D145" s="18"/>
+      <c r="E145" s="19"/>
     </row>
     <row r="146" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B146" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C146" s="15" t="s">
+      <c r="C146" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D146" s="16"/>
-      <c r="E146" s="17"/>
+      <c r="D146" s="24"/>
+      <c r="E146" s="25"/>
     </row>
     <row r="147" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B147" s="1" t="s">
@@ -3012,13 +3026,13 @@
       </c>
     </row>
     <row r="148" spans="2:5" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="B148" s="9">
+      <c r="B148" s="3">
         <v>1</v>
       </c>
-      <c r="C148" s="19" t="s">
+      <c r="C148" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D148" s="19" t="s">
+      <c r="D148" s="7" t="s">
         <v>75</v>
       </c>
       <c r="E148" s="20" t="s">
@@ -3026,76 +3040,76 @@
       </c>
     </row>
     <row r="149" spans="2:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="B149" s="9">
+      <c r="B149" s="3">
         <v>2</v>
       </c>
-      <c r="C149" s="19" t="s">
+      <c r="C149" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D149" s="19" t="s">
+      <c r="D149" s="7" t="s">
         <v>77</v>
       </c>
       <c r="E149" s="22"/>
     </row>
-    <row r="150" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B150" s="9">
+    <row r="150" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B150" s="3">
         <v>3</v>
       </c>
-      <c r="C150" s="19" t="s">
+      <c r="C150" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D150" s="19" t="s">
+      <c r="D150" s="7" t="s">
         <v>79</v>
       </c>
       <c r="E150" s="22"/>
     </row>
-    <row r="151" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B151" s="9">
+    <row r="151" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B151" s="3">
         <v>4</v>
       </c>
-      <c r="C151" s="19" t="s">
+      <c r="C151" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D151" s="19" t="s">
+      <c r="D151" s="7" t="s">
         <v>85</v>
       </c>
       <c r="E151" s="21"/>
     </row>
     <row r="152" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B152" s="5"/>
-      <c r="C152" s="6"/>
-      <c r="D152" s="6"/>
-      <c r="E152" s="7"/>
+      <c r="B152" s="14"/>
+      <c r="C152" s="15"/>
+      <c r="D152" s="15"/>
+      <c r="E152" s="16"/>
     </row>
     <row r="154" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B154" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C154" s="2">
+      <c r="C154" s="17">
         <v>20</v>
       </c>
-      <c r="D154" s="3"/>
-      <c r="E154" s="4"/>
+      <c r="D154" s="18"/>
+      <c r="E154" s="19"/>
     </row>
     <row r="155" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B155" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C155" s="2" t="s">
+      <c r="C155" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D155" s="3"/>
-      <c r="E155" s="4"/>
+      <c r="D155" s="18"/>
+      <c r="E155" s="19"/>
     </row>
     <row r="156" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B156" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C156" s="15" t="s">
+      <c r="C156" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="D156" s="16"/>
-      <c r="E156" s="17"/>
+      <c r="D156" s="24"/>
+      <c r="E156" s="25"/>
     </row>
     <row r="157" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B157" s="1" t="s">
@@ -3111,55 +3125,55 @@
         <v>30</v>
       </c>
     </row>
-    <row r="158" spans="2:5" s="11" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="B158" s="9">
+    <row r="158" spans="2:5" s="5" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="B158" s="3">
         <v>1</v>
       </c>
-      <c r="C158" s="19" t="s">
+      <c r="C158" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D158" s="19" t="s">
+      <c r="D158" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E158" s="19" t="s">
+      <c r="E158" s="8" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="159" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B159" s="5"/>
-      <c r="C159" s="6"/>
-      <c r="D159" s="6"/>
-      <c r="E159" s="7"/>
+      <c r="B159" s="14"/>
+      <c r="C159" s="15"/>
+      <c r="D159" s="15"/>
+      <c r="E159" s="16"/>
     </row>
     <row r="161" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B161" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C161" s="2">
+      <c r="C161" s="17">
         <v>21</v>
       </c>
-      <c r="D161" s="3"/>
-      <c r="E161" s="4"/>
+      <c r="D161" s="18"/>
+      <c r="E161" s="19"/>
     </row>
     <row r="162" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B162" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C162" s="2" t="s">
+      <c r="C162" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D162" s="3"/>
-      <c r="E162" s="4"/>
+      <c r="D162" s="18"/>
+      <c r="E162" s="19"/>
     </row>
     <row r="163" spans="2:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B163" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C163" s="15" t="s">
+      <c r="C163" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="D163" s="16"/>
-      <c r="E163" s="17"/>
+      <c r="D163" s="24"/>
+      <c r="E163" s="25"/>
     </row>
     <row r="164" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B164" s="1" t="s">
@@ -3175,12 +3189,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="165" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B165" s="9"/>
-      <c r="C165" s="19" t="s">
+    <row r="165" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B165" s="3"/>
+      <c r="C165" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D165" s="19" t="s">
+      <c r="D165" s="7" t="s">
         <v>87</v>
       </c>
       <c r="E165" s="20" t="s">
@@ -3188,60 +3202,60 @@
       </c>
     </row>
     <row r="166" spans="2:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="B166" s="9"/>
-      <c r="C166" s="19" t="s">
+      <c r="B166" s="3"/>
+      <c r="C166" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D166" s="19" t="s">
+      <c r="D166" s="7" t="s">
         <v>88</v>
       </c>
       <c r="E166" s="22"/>
     </row>
     <row r="167" spans="2:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="B167" s="9"/>
-      <c r="C167" s="19" t="s">
+      <c r="B167" s="3"/>
+      <c r="C167" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D167" s="19" t="s">
+      <c r="D167" s="7" t="s">
         <v>91</v>
       </c>
       <c r="E167" s="21"/>
     </row>
     <row r="168" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B168" s="5"/>
-      <c r="C168" s="6"/>
-      <c r="D168" s="6"/>
-      <c r="E168" s="7"/>
+      <c r="B168" s="14"/>
+      <c r="C168" s="15"/>
+      <c r="D168" s="15"/>
+      <c r="E168" s="16"/>
     </row>
     <row r="170" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B170" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C170" s="2">
+      <c r="C170" s="17">
         <v>22</v>
       </c>
-      <c r="D170" s="3"/>
-      <c r="E170" s="4"/>
+      <c r="D170" s="18"/>
+      <c r="E170" s="19"/>
     </row>
     <row r="171" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B171" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C171" s="2" t="s">
+      <c r="C171" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D171" s="3"/>
-      <c r="E171" s="4"/>
-    </row>
-    <row r="172" spans="2:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D171" s="18"/>
+      <c r="E171" s="19"/>
+    </row>
+    <row r="172" spans="2:5" s="5" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B172" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C172" s="15" t="s">
+      <c r="C172" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D172" s="16"/>
-      <c r="E172" s="17"/>
+      <c r="D172" s="24"/>
+      <c r="E172" s="25"/>
     </row>
     <row r="173" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B173" s="1" t="s">
@@ -3258,13 +3272,13 @@
       </c>
     </row>
     <row r="174" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B174" s="9">
+      <c r="B174" s="3">
         <v>1</v>
       </c>
-      <c r="C174" s="19" t="s">
+      <c r="C174" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D174" s="19" t="s">
+      <c r="D174" s="7" t="s">
         <v>94</v>
       </c>
       <c r="E174" s="20" t="s">
@@ -3272,88 +3286,88 @@
       </c>
     </row>
     <row r="175" spans="2:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="B175" s="9">
+      <c r="B175" s="3">
         <v>2</v>
       </c>
-      <c r="C175" s="19" t="s">
+      <c r="C175" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D175" s="19" t="s">
+      <c r="D175" s="7" t="s">
         <v>96</v>
       </c>
       <c r="E175" s="22"/>
     </row>
     <row r="176" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B176" s="9">
+      <c r="B176" s="3">
         <v>3</v>
       </c>
-      <c r="C176" s="19" t="s">
+      <c r="C176" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D176" s="19" t="s">
+      <c r="D176" s="7" t="s">
         <v>98</v>
       </c>
       <c r="E176" s="22"/>
     </row>
     <row r="177" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B177" s="9">
+      <c r="B177" s="3">
         <v>4</v>
       </c>
-      <c r="C177" s="19" t="s">
+      <c r="C177" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D177" s="19" t="s">
+      <c r="D177" s="7" t="s">
         <v>100</v>
       </c>
       <c r="E177" s="22"/>
     </row>
     <row r="178" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B178" s="9">
+      <c r="B178" s="3">
         <v>5</v>
       </c>
-      <c r="C178" s="19" t="s">
+      <c r="C178" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D178" s="19" t="s">
+      <c r="D178" s="7" t="s">
         <v>101</v>
       </c>
       <c r="E178" s="21"/>
     </row>
-    <row r="179" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B179" s="5"/>
-      <c r="C179" s="6"/>
-      <c r="D179" s="6"/>
-      <c r="E179" s="7"/>
+    <row r="179" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B179" s="14"/>
+      <c r="C179" s="15"/>
+      <c r="D179" s="15"/>
+      <c r="E179" s="16"/>
     </row>
     <row r="181" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B181" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C181" s="2">
+      <c r="C181" s="17">
         <v>23</v>
       </c>
-      <c r="D181" s="3"/>
-      <c r="E181" s="4"/>
+      <c r="D181" s="18"/>
+      <c r="E181" s="19"/>
     </row>
     <row r="182" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B182" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C182" s="2" t="s">
+      <c r="C182" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="D182" s="3"/>
-      <c r="E182" s="4"/>
-    </row>
-    <row r="183" spans="2:5" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D182" s="18"/>
+      <c r="E182" s="19"/>
+    </row>
+    <row r="183" spans="2:5" s="5" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B183" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C183" s="15" t="s">
+      <c r="C183" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D183" s="16"/>
-      <c r="E183" s="17"/>
+      <c r="D183" s="24"/>
+      <c r="E183" s="25"/>
     </row>
     <row r="184" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B184" s="1" t="s">
@@ -3370,60 +3384,60 @@
       </c>
     </row>
     <row r="185" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B185" s="9">
+      <c r="B185" s="3">
         <v>1</v>
       </c>
-      <c r="C185" s="19" t="s">
+      <c r="C185" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="D185" s="19" t="s">
+      <c r="D185" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="E185" s="19" t="s">
+      <c r="E185" s="8" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="186" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B186" s="5"/>
-      <c r="C186" s="6"/>
-      <c r="D186" s="6"/>
-      <c r="E186" s="7"/>
+    <row r="186" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B186" s="14"/>
+      <c r="C186" s="15"/>
+      <c r="D186" s="15"/>
+      <c r="E186" s="16"/>
     </row>
     <row r="187" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B187" s="8"/>
-      <c r="C187" s="8"/>
-      <c r="D187" s="8"/>
-      <c r="E187" s="8"/>
+      <c r="B187" s="2"/>
+      <c r="C187" s="2"/>
+      <c r="D187" s="2"/>
+      <c r="E187" s="9"/>
     </row>
     <row r="188" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B188" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C188" s="2">
+      <c r="C188" s="17">
         <v>24</v>
       </c>
-      <c r="D188" s="3"/>
-      <c r="E188" s="4"/>
+      <c r="D188" s="18"/>
+      <c r="E188" s="19"/>
     </row>
     <row r="189" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B189" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C189" s="2" t="s">
+      <c r="C189" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D189" s="3"/>
-      <c r="E189" s="4"/>
+      <c r="D189" s="18"/>
+      <c r="E189" s="19"/>
     </row>
     <row r="190" spans="2:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B190" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C190" s="15" t="s">
+      <c r="C190" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D190" s="16"/>
-      <c r="E190" s="17"/>
+      <c r="D190" s="24"/>
+      <c r="E190" s="25"/>
     </row>
     <row r="191" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B191" s="1" t="s">
@@ -3440,54 +3454,54 @@
       </c>
     </row>
     <row r="192" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B192" s="9">
+      <c r="B192" s="3">
         <v>1</v>
       </c>
-      <c r="C192" s="19" t="s">
+      <c r="C192" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D192" s="19" t="s">
+      <c r="D192" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E192" s="19" t="s">
+      <c r="E192" s="8" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="193" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B193" s="5"/>
-      <c r="C193" s="6"/>
-      <c r="D193" s="6"/>
-      <c r="E193" s="7"/>
+    <row r="193" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B193" s="14"/>
+      <c r="C193" s="15"/>
+      <c r="D193" s="15"/>
+      <c r="E193" s="16"/>
     </row>
     <row r="195" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B195" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C195" s="2">
+      <c r="C195" s="17">
         <v>25</v>
       </c>
-      <c r="D195" s="3"/>
-      <c r="E195" s="4"/>
+      <c r="D195" s="18"/>
+      <c r="E195" s="19"/>
     </row>
     <row r="196" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B196" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C196" s="2" t="s">
+      <c r="C196" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D196" s="3"/>
-      <c r="E196" s="4"/>
+      <c r="D196" s="18"/>
+      <c r="E196" s="19"/>
     </row>
     <row r="197" spans="2:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B197" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C197" s="15" t="s">
+      <c r="C197" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D197" s="16"/>
-      <c r="E197" s="17"/>
+      <c r="D197" s="24"/>
+      <c r="E197" s="25"/>
     </row>
     <row r="198" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B198" s="1" t="s">
@@ -3504,54 +3518,54 @@
       </c>
     </row>
     <row r="199" spans="2:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="B199" s="9">
+      <c r="B199" s="3">
         <v>1</v>
       </c>
-      <c r="C199" s="19" t="s">
+      <c r="C199" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D199" s="19" t="s">
+      <c r="D199" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E199" s="19" t="s">
+      <c r="E199" s="8" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="200" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B200" s="5"/>
-      <c r="C200" s="6"/>
-      <c r="D200" s="6"/>
-      <c r="E200" s="7"/>
+    <row r="200" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B200" s="14"/>
+      <c r="C200" s="15"/>
+      <c r="D200" s="15"/>
+      <c r="E200" s="16"/>
     </row>
     <row r="202" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B202" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C202" s="2">
+      <c r="C202" s="17">
         <v>26</v>
       </c>
-      <c r="D202" s="3"/>
-      <c r="E202" s="4"/>
+      <c r="D202" s="18"/>
+      <c r="E202" s="19"/>
     </row>
     <row r="203" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B203" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C203" s="2" t="s">
+      <c r="C203" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D203" s="3"/>
-      <c r="E203" s="4"/>
+      <c r="D203" s="18"/>
+      <c r="E203" s="19"/>
     </row>
     <row r="204" spans="2:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B204" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C204" s="15" t="s">
+      <c r="C204" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="D204" s="16"/>
-      <c r="E204" s="17"/>
+      <c r="D204" s="24"/>
+      <c r="E204" s="25"/>
     </row>
     <row r="205" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B205" s="1" t="s">
@@ -3568,13 +3582,13 @@
       </c>
     </row>
     <row r="206" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B206" s="9">
+      <c r="B206" s="3">
         <v>1</v>
       </c>
-      <c r="C206" s="19" t="s">
+      <c r="C206" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D206" s="19" t="s">
+      <c r="D206" s="7" t="s">
         <v>105</v>
       </c>
       <c r="E206" s="20" t="s">
@@ -3582,64 +3596,64 @@
       </c>
     </row>
     <row r="207" spans="2:5" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="B207" s="9">
+      <c r="B207" s="3">
         <v>2</v>
       </c>
-      <c r="C207" s="19" t="s">
+      <c r="C207" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D207" s="19" t="s">
+      <c r="D207" s="7" t="s">
         <v>107</v>
       </c>
       <c r="E207" s="22"/>
     </row>
     <row r="208" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B208" s="9">
+      <c r="B208" s="3">
         <v>3</v>
       </c>
-      <c r="C208" s="19" t="s">
+      <c r="C208" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D208" s="19" t="s">
+      <c r="D208" s="7" t="s">
         <v>108</v>
       </c>
       <c r="E208" s="21"/>
     </row>
-    <row r="209" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B209" s="5"/>
-      <c r="C209" s="6"/>
-      <c r="D209" s="6"/>
-      <c r="E209" s="7"/>
+    <row r="209" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B209" s="14"/>
+      <c r="C209" s="15"/>
+      <c r="D209" s="15"/>
+      <c r="E209" s="16"/>
     </row>
     <row r="211" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B211" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C211" s="2">
+      <c r="C211" s="17">
         <v>27</v>
       </c>
-      <c r="D211" s="3"/>
-      <c r="E211" s="4"/>
+      <c r="D211" s="18"/>
+      <c r="E211" s="19"/>
     </row>
     <row r="212" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B212" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C212" s="2" t="s">
+      <c r="C212" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="D212" s="3"/>
-      <c r="E212" s="4"/>
+      <c r="D212" s="18"/>
+      <c r="E212" s="19"/>
     </row>
     <row r="213" spans="2:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B213" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C213" s="15" t="s">
+      <c r="C213" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="D213" s="16"/>
-      <c r="E213" s="17"/>
+      <c r="D213" s="24"/>
+      <c r="E213" s="25"/>
     </row>
     <row r="214" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B214" s="1" t="s">
@@ -3656,54 +3670,54 @@
       </c>
     </row>
     <row r="215" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B215" s="9">
+      <c r="B215" s="3">
         <v>1</v>
       </c>
-      <c r="C215" s="19" t="s">
+      <c r="C215" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="D215" s="19" t="s">
+      <c r="D215" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E215" s="19" t="s">
+      <c r="E215" s="8" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="216" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B216" s="5"/>
-      <c r="C216" s="6"/>
-      <c r="D216" s="6"/>
-      <c r="E216" s="7"/>
+    <row r="216" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B216" s="14"/>
+      <c r="C216" s="15"/>
+      <c r="D216" s="15"/>
+      <c r="E216" s="16"/>
     </row>
     <row r="218" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B218" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C218" s="2">
+      <c r="C218" s="17">
         <v>28</v>
       </c>
-      <c r="D218" s="3"/>
-      <c r="E218" s="4"/>
+      <c r="D218" s="18"/>
+      <c r="E218" s="19"/>
     </row>
     <row r="219" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B219" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C219" s="2" t="s">
+      <c r="C219" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D219" s="3"/>
-      <c r="E219" s="4"/>
+      <c r="D219" s="18"/>
+      <c r="E219" s="19"/>
     </row>
     <row r="220" spans="2:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B220" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C220" s="15" t="s">
+      <c r="C220" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="D220" s="16"/>
-      <c r="E220" s="17"/>
+      <c r="D220" s="24"/>
+      <c r="E220" s="25"/>
     </row>
     <row r="221" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B221" s="1" t="s">
@@ -3720,54 +3734,54 @@
       </c>
     </row>
     <row r="222" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B222" s="9">
+      <c r="B222" s="3">
         <v>1</v>
       </c>
-      <c r="C222" s="19" t="s">
+      <c r="C222" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D222" s="19" t="s">
+      <c r="D222" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="E222" s="19" t="s">
+      <c r="E222" s="8" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="223" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B223" s="5"/>
-      <c r="C223" s="6"/>
-      <c r="D223" s="6"/>
-      <c r="E223" s="7"/>
+    <row r="223" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B223" s="14"/>
+      <c r="C223" s="15"/>
+      <c r="D223" s="15"/>
+      <c r="E223" s="16"/>
     </row>
     <row r="225" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B225" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C225" s="2">
+      <c r="C225" s="17">
         <v>29</v>
       </c>
-      <c r="D225" s="3"/>
-      <c r="E225" s="4"/>
+      <c r="D225" s="18"/>
+      <c r="E225" s="19"/>
     </row>
     <row r="226" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B226" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C226" s="2" t="s">
+      <c r="C226" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D226" s="3"/>
-      <c r="E226" s="4"/>
+      <c r="D226" s="18"/>
+      <c r="E226" s="19"/>
     </row>
     <row r="227" spans="2:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B227" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C227" s="15" t="s">
+      <c r="C227" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="D227" s="16"/>
-      <c r="E227" s="17"/>
+      <c r="D227" s="24"/>
+      <c r="E227" s="25"/>
     </row>
     <row r="228" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B228" s="1" t="s">
@@ -3784,54 +3798,54 @@
       </c>
     </row>
     <row r="229" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B229" s="9">
+      <c r="B229" s="3">
         <v>1</v>
       </c>
-      <c r="C229" s="19" t="s">
+      <c r="C229" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D229" s="19" t="s">
+      <c r="D229" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="E229" s="19" t="s">
+      <c r="E229" s="8" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="230" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B230" s="5"/>
-      <c r="C230" s="6"/>
-      <c r="D230" s="6"/>
-      <c r="E230" s="7"/>
+    <row r="230" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B230" s="14"/>
+      <c r="C230" s="15"/>
+      <c r="D230" s="15"/>
+      <c r="E230" s="16"/>
     </row>
     <row r="232" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B232" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C232" s="2">
+      <c r="C232" s="17">
         <v>30</v>
       </c>
-      <c r="D232" s="3"/>
-      <c r="E232" s="4"/>
+      <c r="D232" s="18"/>
+      <c r="E232" s="19"/>
     </row>
     <row r="233" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B233" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C233" s="2" t="s">
+      <c r="C233" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="D233" s="3"/>
-      <c r="E233" s="4"/>
+      <c r="D233" s="18"/>
+      <c r="E233" s="19"/>
     </row>
     <row r="234" spans="2:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B234" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C234" s="15" t="s">
+      <c r="C234" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="D234" s="16"/>
-      <c r="E234" s="17"/>
+      <c r="D234" s="24"/>
+      <c r="E234" s="25"/>
     </row>
     <row r="235" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B235" s="1" t="s">
@@ -3848,13 +3862,13 @@
       </c>
     </row>
     <row r="236" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B236" s="9">
+      <c r="B236" s="3">
         <v>1</v>
       </c>
-      <c r="C236" s="19" t="s">
+      <c r="C236" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D236" s="19" t="s">
+      <c r="D236" s="7" t="s">
         <v>105</v>
       </c>
       <c r="E236" s="20" t="s">
@@ -3862,88 +3876,88 @@
       </c>
     </row>
     <row r="237" spans="2:5" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="B237" s="9">
+      <c r="B237" s="3">
         <v>2</v>
       </c>
-      <c r="C237" s="19" t="s">
+      <c r="C237" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D237" s="19" t="s">
+      <c r="D237" s="7" t="s">
         <v>107</v>
       </c>
       <c r="E237" s="22"/>
     </row>
     <row r="238" spans="2:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="B238" s="9">
+      <c r="B238" s="3">
         <v>3</v>
       </c>
-      <c r="C238" s="19" t="s">
+      <c r="C238" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="D238" s="19" t="s">
+      <c r="D238" s="7" t="s">
         <v>118</v>
       </c>
       <c r="E238" s="22"/>
     </row>
     <row r="239" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B239" s="9">
+      <c r="B239" s="3">
         <v>4</v>
       </c>
-      <c r="C239" s="19" t="s">
+      <c r="C239" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D239" s="19" t="s">
+      <c r="D239" s="7" t="s">
         <v>119</v>
       </c>
       <c r="E239" s="22"/>
     </row>
     <row r="240" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B240" s="9">
+      <c r="B240" s="3">
         <v>5</v>
       </c>
-      <c r="C240" s="19" t="s">
+      <c r="C240" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D240" s="19" t="s">
+      <c r="D240" s="7" t="s">
         <v>108</v>
       </c>
       <c r="E240" s="21"/>
     </row>
-    <row r="241" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B241" s="5"/>
-      <c r="C241" s="6"/>
-      <c r="D241" s="6"/>
-      <c r="E241" s="7"/>
+    <row r="241" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B241" s="14"/>
+      <c r="C241" s="15"/>
+      <c r="D241" s="15"/>
+      <c r="E241" s="16"/>
     </row>
     <row r="243" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B243" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C243" s="2">
+      <c r="C243" s="17">
         <v>31</v>
       </c>
-      <c r="D243" s="3"/>
-      <c r="E243" s="4"/>
+      <c r="D243" s="18"/>
+      <c r="E243" s="19"/>
     </row>
     <row r="244" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B244" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C244" s="2" t="s">
+      <c r="C244" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D244" s="3"/>
-      <c r="E244" s="4"/>
+      <c r="D244" s="18"/>
+      <c r="E244" s="19"/>
     </row>
     <row r="245" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B245" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C245" s="15" t="s">
+      <c r="C245" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="D245" s="16"/>
-      <c r="E245" s="17"/>
+      <c r="D245" s="24"/>
+      <c r="E245" s="25"/>
     </row>
     <row r="246" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B246" s="1" t="s">
@@ -3960,13 +3974,13 @@
       </c>
     </row>
     <row r="247" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B247" s="9">
+      <c r="B247" s="3">
         <v>1</v>
       </c>
-      <c r="C247" s="19" t="s">
+      <c r="C247" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D247" s="19" t="s">
+      <c r="D247" s="7" t="s">
         <v>105</v>
       </c>
       <c r="E247" s="20" t="s">
@@ -3974,76 +3988,76 @@
       </c>
     </row>
     <row r="248" spans="2:5" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="B248" s="9">
+      <c r="B248" s="3">
         <v>2</v>
       </c>
-      <c r="C248" s="19" t="s">
+      <c r="C248" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D248" s="19" t="s">
+      <c r="D248" s="7" t="s">
         <v>107</v>
       </c>
       <c r="E248" s="22"/>
     </row>
     <row r="249" spans="2:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="B249" s="9">
+      <c r="B249" s="3">
         <v>3</v>
       </c>
-      <c r="C249" s="19" t="s">
+      <c r="C249" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="D249" s="19" t="s">
+      <c r="D249" s="7" t="s">
         <v>118</v>
       </c>
       <c r="E249" s="22"/>
     </row>
     <row r="250" spans="2:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="B250" s="9">
+      <c r="B250" s="3">
         <v>4</v>
       </c>
-      <c r="C250" s="19" t="s">
+      <c r="C250" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D250" s="19" t="s">
+      <c r="D250" s="7" t="s">
         <v>121</v>
       </c>
       <c r="E250" s="21"/>
     </row>
-    <row r="251" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B251" s="5"/>
-      <c r="C251" s="6"/>
-      <c r="D251" s="6"/>
-      <c r="E251" s="7"/>
+    <row r="251" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B251" s="14"/>
+      <c r="C251" s="15"/>
+      <c r="D251" s="15"/>
+      <c r="E251" s="16"/>
     </row>
     <row r="253" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B253" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C253" s="2">
+      <c r="C253" s="17">
         <v>32</v>
       </c>
-      <c r="D253" s="3"/>
-      <c r="E253" s="4"/>
+      <c r="D253" s="18"/>
+      <c r="E253" s="19"/>
     </row>
     <row r="254" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B254" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C254" s="2" t="s">
+      <c r="C254" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D254" s="3"/>
-      <c r="E254" s="4"/>
+      <c r="D254" s="18"/>
+      <c r="E254" s="19"/>
     </row>
     <row r="255" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B255" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C255" s="15" t="s">
+      <c r="C255" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="D255" s="16"/>
-      <c r="E255" s="17"/>
+      <c r="D255" s="24"/>
+      <c r="E255" s="25"/>
     </row>
     <row r="256" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B256" s="1" t="s">
@@ -4060,78 +4074,78 @@
       </c>
     </row>
     <row r="257" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B257" s="9">
+      <c r="B257" s="3">
         <v>1</v>
       </c>
-      <c r="C257" s="19" t="s">
+      <c r="C257" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="D257" s="19" t="s">
+      <c r="D257" s="7" t="s">
         <v>126</v>
       </c>
       <c r="E257" s="20" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="258" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B258" s="9">
+    <row r="258" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B258" s="3">
         <v>2</v>
       </c>
-      <c r="C258" s="19" t="s">
+      <c r="C258" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D258" s="19" t="s">
+      <c r="D258" s="7" t="s">
         <v>108</v>
       </c>
       <c r="E258" s="22"/>
     </row>
-    <row r="259" spans="2:5" s="11" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B259" s="9">
+    <row r="259" spans="2:5" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B259" s="3">
         <v>3</v>
       </c>
-      <c r="C259" s="19" t="s">
+      <c r="C259" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D259" s="19" t="s">
+      <c r="D259" s="7" t="s">
         <v>127</v>
       </c>
       <c r="E259" s="21"/>
     </row>
     <row r="260" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B260" s="5"/>
-      <c r="C260" s="6"/>
-      <c r="D260" s="6"/>
-      <c r="E260" s="7"/>
+      <c r="B260" s="14"/>
+      <c r="C260" s="15"/>
+      <c r="D260" s="15"/>
+      <c r="E260" s="16"/>
     </row>
     <row r="262" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B262" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C262" s="2">
+      <c r="C262" s="17">
         <v>33</v>
       </c>
-      <c r="D262" s="3"/>
-      <c r="E262" s="4"/>
+      <c r="D262" s="18"/>
+      <c r="E262" s="19"/>
     </row>
     <row r="263" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B263" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C263" s="2" t="s">
+      <c r="C263" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="D263" s="3"/>
-      <c r="E263" s="4"/>
+      <c r="D263" s="18"/>
+      <c r="E263" s="19"/>
     </row>
     <row r="264" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B264" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C264" s="15" t="s">
+      <c r="C264" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="D264" s="16"/>
-      <c r="E264" s="17"/>
+      <c r="D264" s="24"/>
+      <c r="E264" s="25"/>
     </row>
     <row r="265" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B265" s="1" t="s">
@@ -4147,67 +4161,67 @@
         <v>30</v>
       </c>
     </row>
-    <row r="266" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B266" s="9">
+    <row r="266" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B266" s="3">
         <v>1</v>
       </c>
-      <c r="C266" s="19" t="s">
+      <c r="C266" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D266" s="19" t="s">
+      <c r="D266" s="7" t="s">
         <v>108</v>
       </c>
       <c r="E266" s="22" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="267" spans="2:5" s="11" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B267" s="9">
+    <row r="267" spans="2:5" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B267" s="3">
         <v>2</v>
       </c>
-      <c r="C267" s="19" t="s">
+      <c r="C267" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D267" s="19" t="s">
+      <c r="D267" s="7" t="s">
         <v>246</v>
       </c>
       <c r="E267" s="21"/>
     </row>
     <row r="268" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B268" s="5"/>
-      <c r="C268" s="6"/>
-      <c r="D268" s="6"/>
-      <c r="E268" s="7"/>
+      <c r="B268" s="14"/>
+      <c r="C268" s="15"/>
+      <c r="D268" s="15"/>
+      <c r="E268" s="16"/>
     </row>
     <row r="270" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B270" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C270" s="2">
+      <c r="C270" s="17">
         <v>34</v>
       </c>
-      <c r="D270" s="3"/>
-      <c r="E270" s="4"/>
+      <c r="D270" s="18"/>
+      <c r="E270" s="19"/>
     </row>
     <row r="271" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B271" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C271" s="2" t="s">
+      <c r="C271" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D271" s="3"/>
-      <c r="E271" s="4"/>
+      <c r="D271" s="18"/>
+      <c r="E271" s="19"/>
     </row>
     <row r="272" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B272" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C272" s="15" t="s">
+      <c r="C272" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="D272" s="16"/>
-      <c r="E272" s="17"/>
+      <c r="D272" s="24"/>
+      <c r="E272" s="25"/>
     </row>
     <row r="273" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B273" s="1" t="s">
@@ -4223,55 +4237,55 @@
         <v>30</v>
       </c>
     </row>
-    <row r="274" spans="2:5" s="11" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B274" s="9">
+    <row r="274" spans="2:5" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B274" s="3">
         <v>1</v>
       </c>
-      <c r="C274" s="19" t="s">
+      <c r="C274" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D274" s="19" t="s">
+      <c r="D274" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="E274" s="19" t="s">
+      <c r="E274" s="8" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="275" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B275" s="5"/>
-      <c r="C275" s="6"/>
-      <c r="D275" s="6"/>
-      <c r="E275" s="7"/>
+      <c r="B275" s="14"/>
+      <c r="C275" s="15"/>
+      <c r="D275" s="15"/>
+      <c r="E275" s="16"/>
     </row>
     <row r="277" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B277" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C277" s="2">
+      <c r="C277" s="17">
         <v>35</v>
       </c>
-      <c r="D277" s="3"/>
-      <c r="E277" s="4"/>
+      <c r="D277" s="18"/>
+      <c r="E277" s="19"/>
     </row>
     <row r="278" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B278" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C278" s="2" t="s">
+      <c r="C278" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D278" s="3"/>
-      <c r="E278" s="4"/>
+      <c r="D278" s="18"/>
+      <c r="E278" s="19"/>
     </row>
     <row r="279" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B279" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C279" s="15" t="s">
+      <c r="C279" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="D279" s="16"/>
-      <c r="E279" s="17"/>
+      <c r="D279" s="24"/>
+      <c r="E279" s="25"/>
     </row>
     <row r="280" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B280" s="1" t="s">
@@ -4287,55 +4301,55 @@
         <v>30</v>
       </c>
     </row>
-    <row r="281" spans="2:5" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B281" s="9">
+    <row r="281" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B281" s="3">
         <v>1</v>
       </c>
-      <c r="C281" s="19" t="s">
+      <c r="C281" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D281" s="19" t="s">
+      <c r="D281" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="E281" s="19" t="s">
+      <c r="E281" s="8" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="282" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B282" s="5"/>
-      <c r="C282" s="6"/>
-      <c r="D282" s="6"/>
-      <c r="E282" s="7"/>
+      <c r="B282" s="14"/>
+      <c r="C282" s="15"/>
+      <c r="D282" s="15"/>
+      <c r="E282" s="16"/>
     </row>
     <row r="284" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B284" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C284" s="2">
+      <c r="C284" s="17">
         <v>36</v>
       </c>
-      <c r="D284" s="3"/>
-      <c r="E284" s="4"/>
+      <c r="D284" s="18"/>
+      <c r="E284" s="19"/>
     </row>
     <row r="285" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B285" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C285" s="2" t="s">
+      <c r="C285" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D285" s="3"/>
-      <c r="E285" s="4"/>
+      <c r="D285" s="18"/>
+      <c r="E285" s="19"/>
     </row>
     <row r="286" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B286" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C286" s="15" t="s">
+      <c r="C286" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D286" s="16"/>
-      <c r="E286" s="17"/>
+      <c r="D286" s="24"/>
+      <c r="E286" s="25"/>
     </row>
     <row r="287" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B287" s="1" t="s">
@@ -4352,54 +4366,54 @@
       </c>
     </row>
     <row r="288" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B288" s="9">
+      <c r="B288" s="3">
         <v>1</v>
       </c>
-      <c r="C288" s="19" t="s">
+      <c r="C288" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D288" s="19" t="s">
+      <c r="D288" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="E288" s="19" t="s">
+      <c r="E288" s="8" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="289" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B289" s="5"/>
-      <c r="C289" s="6"/>
-      <c r="D289" s="6"/>
-      <c r="E289" s="7"/>
+      <c r="B289" s="14"/>
+      <c r="C289" s="15"/>
+      <c r="D289" s="15"/>
+      <c r="E289" s="16"/>
     </row>
     <row r="291" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B291" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C291" s="2">
+      <c r="C291" s="17">
         <v>37</v>
       </c>
-      <c r="D291" s="3"/>
-      <c r="E291" s="4"/>
+      <c r="D291" s="18"/>
+      <c r="E291" s="19"/>
     </row>
     <row r="292" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B292" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C292" s="2" t="s">
+      <c r="C292" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="D292" s="3"/>
-      <c r="E292" s="4"/>
+      <c r="D292" s="18"/>
+      <c r="E292" s="19"/>
     </row>
     <row r="293" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B293" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C293" s="15" t="s">
+      <c r="C293" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D293" s="16"/>
-      <c r="E293" s="17"/>
+      <c r="D293" s="24"/>
+      <c r="E293" s="25"/>
     </row>
     <row r="294" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B294" s="1" t="s">
@@ -4416,54 +4430,54 @@
       </c>
     </row>
     <row r="295" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B295" s="9">
+      <c r="B295" s="3">
         <v>1</v>
       </c>
-      <c r="C295" s="19" t="s">
+      <c r="C295" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="D295" s="19" t="s">
+      <c r="D295" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="E295" s="19" t="s">
+      <c r="E295" s="8" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="296" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B296" s="5"/>
-      <c r="C296" s="6"/>
-      <c r="D296" s="6"/>
-      <c r="E296" s="7"/>
+      <c r="B296" s="14"/>
+      <c r="C296" s="15"/>
+      <c r="D296" s="15"/>
+      <c r="E296" s="16"/>
     </row>
     <row r="298" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B298" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C298" s="2">
+      <c r="C298" s="17">
         <v>38</v>
       </c>
-      <c r="D298" s="3"/>
-      <c r="E298" s="4"/>
+      <c r="D298" s="18"/>
+      <c r="E298" s="19"/>
     </row>
     <row r="299" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B299" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C299" s="2" t="s">
+      <c r="C299" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="D299" s="3"/>
-      <c r="E299" s="4"/>
+      <c r="D299" s="18"/>
+      <c r="E299" s="19"/>
     </row>
     <row r="300" spans="2:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B300" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C300" s="15" t="s">
+      <c r="C300" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="D300" s="16"/>
-      <c r="E300" s="17"/>
+      <c r="D300" s="24"/>
+      <c r="E300" s="25"/>
     </row>
     <row r="301" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B301" s="1" t="s">
@@ -4480,51 +4494,71 @@
       </c>
     </row>
     <row r="302" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B302" s="9">
+      <c r="B302" s="3">
         <v>1</v>
       </c>
-      <c r="C302" s="19" t="s">
+      <c r="C302" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D302" s="19" t="s">
+      <c r="D302" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="E302" s="19" t="s">
+      <c r="E302" s="8" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="303" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B303" s="5"/>
-      <c r="C303" s="6"/>
-      <c r="D303" s="6"/>
-      <c r="E303" s="7"/>
+      <c r="B303" s="14"/>
+      <c r="C303" s="15"/>
+      <c r="D303" s="15"/>
+      <c r="E303" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="172">
-    <mergeCell ref="C262:E262"/>
-    <mergeCell ref="C263:E263"/>
-    <mergeCell ref="C264:E264"/>
-    <mergeCell ref="E266:E267"/>
-    <mergeCell ref="B268:E268"/>
     <mergeCell ref="B303:E303"/>
     <mergeCell ref="C300:E300"/>
     <mergeCell ref="C299:E299"/>
     <mergeCell ref="C298:E298"/>
+    <mergeCell ref="B296:E296"/>
+    <mergeCell ref="C293:E293"/>
+    <mergeCell ref="C292:E292"/>
+    <mergeCell ref="C291:E291"/>
+    <mergeCell ref="C279:E279"/>
+    <mergeCell ref="B282:E282"/>
+    <mergeCell ref="C284:E284"/>
+    <mergeCell ref="C285:E285"/>
+    <mergeCell ref="C286:E286"/>
+    <mergeCell ref="B289:E289"/>
+    <mergeCell ref="C232:E232"/>
+    <mergeCell ref="C233:E233"/>
+    <mergeCell ref="C234:E234"/>
+    <mergeCell ref="B241:E241"/>
+    <mergeCell ref="E236:E240"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C226:E226"/>
+    <mergeCell ref="C197:E197"/>
+    <mergeCell ref="B200:E200"/>
+    <mergeCell ref="C202:E202"/>
+    <mergeCell ref="C203:E203"/>
+    <mergeCell ref="C204:E204"/>
+    <mergeCell ref="B209:E209"/>
+    <mergeCell ref="C227:E227"/>
+    <mergeCell ref="B230:E230"/>
+    <mergeCell ref="C218:E218"/>
+    <mergeCell ref="C219:E219"/>
+    <mergeCell ref="C220:E220"/>
+    <mergeCell ref="B223:E223"/>
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="E21:E22"/>
     <mergeCell ref="E29:E31"/>
     <mergeCell ref="E45:E46"/>
     <mergeCell ref="E60:E62"/>
-    <mergeCell ref="C232:E232"/>
-    <mergeCell ref="C233:E233"/>
-    <mergeCell ref="C234:E234"/>
-    <mergeCell ref="B241:E241"/>
-    <mergeCell ref="B296:E296"/>
-    <mergeCell ref="C293:E293"/>
-    <mergeCell ref="C292:E292"/>
-    <mergeCell ref="C291:E291"/>
-    <mergeCell ref="E236:E240"/>
-    <mergeCell ref="E247:E250"/>
+    <mergeCell ref="C188:E188"/>
+    <mergeCell ref="C189:E189"/>
+    <mergeCell ref="C190:E190"/>
+    <mergeCell ref="B193:E193"/>
+    <mergeCell ref="C195:E195"/>
+    <mergeCell ref="C196:E196"/>
     <mergeCell ref="C183:E183"/>
     <mergeCell ref="B186:E186"/>
     <mergeCell ref="C211:E211"/>
@@ -4542,17 +4576,6 @@
     <mergeCell ref="E116:E118"/>
     <mergeCell ref="E125:E126"/>
     <mergeCell ref="E133:E134"/>
-    <mergeCell ref="C279:E279"/>
-    <mergeCell ref="B282:E282"/>
-    <mergeCell ref="C284:E284"/>
-    <mergeCell ref="C285:E285"/>
-    <mergeCell ref="C286:E286"/>
-    <mergeCell ref="B289:E289"/>
-    <mergeCell ref="C270:E270"/>
-    <mergeCell ref="C271:E271"/>
-    <mergeCell ref="C272:E272"/>
-    <mergeCell ref="B275:E275"/>
-    <mergeCell ref="C277:E277"/>
     <mergeCell ref="C278:E278"/>
     <mergeCell ref="C245:E245"/>
     <mergeCell ref="B251:E251"/>
@@ -4563,26 +4586,17 @@
     <mergeCell ref="E257:E259"/>
     <mergeCell ref="C243:E243"/>
     <mergeCell ref="C244:E244"/>
-    <mergeCell ref="C227:E227"/>
-    <mergeCell ref="B230:E230"/>
-    <mergeCell ref="C218:E218"/>
-    <mergeCell ref="C219:E219"/>
-    <mergeCell ref="C220:E220"/>
-    <mergeCell ref="B223:E223"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C226:E226"/>
-    <mergeCell ref="C197:E197"/>
-    <mergeCell ref="B200:E200"/>
-    <mergeCell ref="C202:E202"/>
-    <mergeCell ref="C203:E203"/>
-    <mergeCell ref="C204:E204"/>
-    <mergeCell ref="B209:E209"/>
-    <mergeCell ref="C188:E188"/>
-    <mergeCell ref="C189:E189"/>
-    <mergeCell ref="C190:E190"/>
-    <mergeCell ref="B193:E193"/>
-    <mergeCell ref="C195:E195"/>
-    <mergeCell ref="C196:E196"/>
+    <mergeCell ref="E247:E250"/>
+    <mergeCell ref="C262:E262"/>
+    <mergeCell ref="C263:E263"/>
+    <mergeCell ref="C264:E264"/>
+    <mergeCell ref="E266:E267"/>
+    <mergeCell ref="B268:E268"/>
+    <mergeCell ref="C270:E270"/>
+    <mergeCell ref="C271:E271"/>
+    <mergeCell ref="C272:E272"/>
+    <mergeCell ref="B275:E275"/>
+    <mergeCell ref="C277:E277"/>
     <mergeCell ref="C163:E163"/>
     <mergeCell ref="B168:E168"/>
     <mergeCell ref="C170:E170"/>
@@ -4680,22 +4694,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D71"/>
+  <dimension ref="B2:E71"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" style="8"/>
-    <col min="2" max="2" width="4.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="2.5703125" style="8"/>
+    <col min="1" max="1" width="2.5703125" style="2"/>
+    <col min="2" max="2" width="4.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="2.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>32</v>
       </c>
@@ -4705,767 +4720,841 @@
       <c r="D2" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="E2" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+      <c r="E3" s="26"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
+      <c r="E4" s="26"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
+      <c r="E5" s="26"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
+      <c r="E6" s="26"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+      <c r="E7" s="26"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
+      <c r="E8" s="26"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
+      <c r="E9" s="26"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="7" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="9" t="s">
+      <c r="E10" s="26"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="7" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="s">
+      <c r="E11" s="26"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="7" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="9" t="s">
+      <c r="E12" s="26"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="7" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="9" t="s">
+      <c r="E13" s="26"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="7" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="9" t="s">
+      <c r="E14" s="26"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="7" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="9" t="s">
+      <c r="E15" s="26"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="7" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="9" t="s">
+      <c r="E16" s="26"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="7" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="9" t="s">
+      <c r="E17" s="26"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="7" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="9" t="s">
+      <c r="E18" s="26"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="7" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="9" t="s">
+      <c r="E19" s="26"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="7" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="9" t="s">
+      <c r="E20" s="26"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="7" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="9" t="s">
+      <c r="E21" s="26"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="9" t="s">
+      <c r="E22" s="26"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="7" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="9" t="s">
+      <c r="E23" s="26"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="7" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="9" t="s">
+      <c r="E24" s="26"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C25" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="7" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="9" t="s">
+      <c r="E25" s="26"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="C26" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="7" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="9" t="s">
+      <c r="E26" s="26"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="C27" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="7" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="9" t="s">
+      <c r="E27" s="26"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="7" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="9" t="s">
+      <c r="E28" s="26"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="C29" s="19" t="s">
+      <c r="C29" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D29" s="7" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="9" t="s">
+      <c r="E29" s="26"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="C30" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="D30" s="19" t="s">
+      <c r="D30" s="7" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="9" t="s">
+      <c r="E30" s="26"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C31" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="7" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="9" t="s">
+      <c r="E31" s="26"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="C32" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="D32" s="19" t="s">
+      <c r="D32" s="7" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="9" t="s">
+      <c r="E32" s="26"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="C33" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="D33" s="19" t="s">
+      <c r="D33" s="7" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="9" t="s">
+      <c r="E33" s="26"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="C34" s="19" t="s">
+      <c r="C34" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="D34" s="19" t="s">
+      <c r="D34" s="7" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="9" t="s">
+      <c r="E34" s="26"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C35" s="19" t="s">
+      <c r="C35" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="D35" s="19" t="s">
+      <c r="D35" s="7" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="9" t="s">
+      <c r="E35" s="26"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="C36" s="19" t="s">
+      <c r="C36" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D36" s="7" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="9" t="s">
+      <c r="E36" s="26"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="C37" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="D37" s="19" t="s">
+      <c r="D37" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="9" t="s">
+      <c r="E37" s="26"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="C38" s="19" t="s">
+      <c r="C38" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="9" t="s">
+      <c r="E38" s="26"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="C39" s="19" t="s">
+      <c r="C39" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="D39" s="19" t="s">
+      <c r="D39" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="9" t="s">
+      <c r="E39" s="26"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="C40" s="19" t="s">
+      <c r="C40" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="D40" s="19" t="s">
+      <c r="D40" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="9" t="s">
+      <c r="E40" s="26"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C41" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="D41" s="19" t="s">
+      <c r="D41" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="9" t="s">
+      <c r="E41" s="26"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="C42" s="19" t="s">
+      <c r="C42" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="D42" s="19" t="s">
+      <c r="D42" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="9" t="s">
+      <c r="E42" s="26"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="C43" s="19" t="s">
+      <c r="C43" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="D43" s="19" t="s">
+      <c r="D43" s="7" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="9" t="s">
+      <c r="E43" s="26"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C44" s="19" t="s">
+      <c r="C44" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="D44" s="19" t="s">
+      <c r="D44" s="7" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="9" t="s">
+      <c r="E44" s="26"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="C45" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="D45" s="19" t="s">
+      <c r="D45" s="7" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="9" t="s">
+      <c r="E45" s="26"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="C46" s="19" t="s">
+      <c r="C46" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="D46" s="19" t="s">
+      <c r="D46" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="9" t="s">
+      <c r="E46" s="26"/>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="C47" s="19" t="s">
+      <c r="C47" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="D47" s="19" t="s">
+      <c r="D47" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="9" t="s">
+      <c r="E47" s="26"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="C48" s="19" t="s">
+      <c r="C48" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="D48" s="19" t="s">
+      <c r="D48" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="9" t="s">
+      <c r="E48" s="26"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="C49" s="19" t="s">
+      <c r="C49" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="D49" s="19" t="s">
+      <c r="D49" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="9" t="s">
+      <c r="E49" s="26"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="C50" s="19" t="s">
+      <c r="C50" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="D50" s="19" t="s">
+      <c r="D50" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="9" t="s">
+      <c r="E50" s="26"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="C51" s="19" t="s">
+      <c r="C51" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="D51" s="19" t="s">
+      <c r="D51" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="9" t="s">
+      <c r="E51" s="26"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="C52" s="19" t="s">
+      <c r="C52" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="D52" s="19" t="s">
+      <c r="D52" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="9" t="s">
+      <c r="E52" s="26"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="C53" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="D53" s="19" t="s">
+      <c r="D53" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="9" t="s">
+      <c r="E53" s="26"/>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="C54" s="19" t="s">
+      <c r="C54" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="D54" s="19" t="s">
+      <c r="D54" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="9" t="s">
+      <c r="E54" s="26"/>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="C55" s="19" t="s">
+      <c r="C55" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="D55" s="19" t="s">
+      <c r="D55" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="9" t="s">
+      <c r="E55" s="26"/>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="C56" s="19" t="s">
+      <c r="C56" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="D56" s="19" t="s">
+      <c r="D56" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="9" t="s">
+      <c r="E56" s="26"/>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C57" s="19" t="s">
+      <c r="C57" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="D57" s="19" t="s">
+      <c r="D57" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="9" t="s">
+      <c r="E57" s="26"/>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B58" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="C58" s="19" t="s">
+      <c r="C58" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="D58" s="19" t="s">
+      <c r="D58" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="9" t="s">
+      <c r="E58" s="26"/>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B59" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="C59" s="19" t="s">
+      <c r="C59" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="D59" s="19" t="s">
+      <c r="D59" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B60" s="9" t="s">
+      <c r="E59" s="26"/>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="C60" s="19" t="s">
+      <c r="C60" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="D60" s="19" t="s">
+      <c r="D60" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="9" t="s">
+      <c r="E60" s="26"/>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B61" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="C61" s="19" t="s">
+      <c r="C61" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="D61" s="19" t="s">
+      <c r="D61" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="9" t="s">
+      <c r="E61" s="26"/>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B62" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="C62" s="19" t="s">
+      <c r="C62" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="D62" s="19" t="s">
+      <c r="D62" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="9" t="s">
+      <c r="E62" s="26"/>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B63" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="C63" s="19" t="s">
+      <c r="C63" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="D63" s="19" t="s">
+      <c r="D63" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B64" s="9" t="s">
+      <c r="E63" s="26"/>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B64" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="C64" s="19" t="s">
+      <c r="C64" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D64" s="19" t="s">
+      <c r="D64" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="9" t="s">
+      <c r="E64" s="26"/>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B65" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="C65" s="19" t="s">
+      <c r="C65" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="D65" s="19" t="s">
+      <c r="D65" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="9" t="s">
+      <c r="E65" s="26"/>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="C66" s="19" t="s">
+      <c r="C66" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D66" s="19" t="s">
+      <c r="D66" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="9" t="s">
+      <c r="E66" s="26"/>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="C67" s="19" t="s">
+      <c r="C67" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="D67" s="19" t="s">
+      <c r="D67" s="7" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="9" t="s">
+      <c r="E67" s="26"/>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B68" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="C68" s="19" t="s">
+      <c r="C68" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="D68" s="19" t="s">
+      <c r="D68" s="7" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="9" t="s">
+      <c r="E68" s="26"/>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B69" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="C69" s="19" t="s">
+      <c r="C69" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="D69" s="19" t="s">
+      <c r="D69" s="7" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="9" t="s">
+      <c r="E69" s="26"/>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B70" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="C70" s="19" t="s">
+      <c r="C70" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="D70" s="19" t="s">
+      <c r="D70" s="7" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="9" t="s">
+      <c r="E70" s="26"/>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B71" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="C71" s="19" t="s">
+      <c r="C71" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="D71" s="19" t="s">
+      <c r="D71" s="7" t="s">
         <v>142</v>
       </c>
+      <c r="E71" s="26"/>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commitando os casos de teste feitos pelo Carlos - Issue #32
</commit_message>
<xml_diff>
--- a/War/Testes/Casos de Teste/Casos de Teste.xlsx
+++ b/War/Testes/Casos de Teste/Casos de Teste.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Teste" sheetId="2" r:id="rId1"/>
@@ -928,8 +928,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1276,15 +1276,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1292,6 +1284,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1306,22 +1307,21 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="11" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="12" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="12" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="Bom 2" xfId="2"/>
@@ -1431,7 +1431,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1466,7 +1465,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -1642,14 +1640,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:E303"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2" style="2" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" style="4" bestFit="1" customWidth="1"/>
@@ -1659,35 +1657,35 @@
     <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5">
       <c r="B2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="18">
         <v>1</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D2" s="19"/>
+      <c r="E2" s="20"/>
+    </row>
+    <row r="3" spans="2:5">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="2:5">
       <c r="B4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="24"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26"/>
+    </row>
+    <row r="5" spans="2:5">
       <c r="B5" s="1" t="s">
         <v>27</v>
       </c>
@@ -1701,7 +1699,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B6" s="3">
         <v>1</v>
       </c>
@@ -1715,41 +1713,41 @@
         <v>262</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5">
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
+    </row>
+    <row r="9" spans="2:5">
       <c r="B9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="18">
         <v>2</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="19"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="19"/>
+      <c r="E9" s="20"/>
+    </row>
+    <row r="10" spans="2:5">
       <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="19"/>
+      <c r="E10" s="20"/>
+    </row>
+    <row r="11" spans="2:5">
       <c r="B11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="24"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="26"/>
+    </row>
+    <row r="12" spans="2:5">
       <c r="B12" s="1" t="s">
         <v>27</v>
       </c>
@@ -1763,7 +1761,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B13" s="3">
         <v>1</v>
       </c>
@@ -1773,11 +1771,11 @@
       <c r="D13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="21" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="14" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B14" s="3">
         <v>2</v>
       </c>
@@ -1787,43 +1785,43 @@
       <c r="D14" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="21"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="16"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="23"/>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="14"/>
+    </row>
+    <row r="17" spans="2:5">
       <c r="B17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C17" s="18">
         <v>3</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="19"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="19"/>
+      <c r="E17" s="20"/>
+    </row>
+    <row r="18" spans="2:5">
       <c r="B18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="19"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="19"/>
+      <c r="E18" s="20"/>
+    </row>
+    <row r="19" spans="2:5">
       <c r="B19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="13"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="24"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="26"/>
+    </row>
+    <row r="20" spans="2:5">
       <c r="B20" s="1" t="s">
         <v>27</v>
       </c>
@@ -1837,7 +1835,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B21" s="3">
         <v>1</v>
       </c>
@@ -1847,11 +1845,11 @@
       <c r="D21" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="21" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="22" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B22" s="3">
         <v>2</v>
       </c>
@@ -1861,43 +1859,43 @@
       <c r="D22" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="21"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="14"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="16"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="23"/>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" s="12"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="14"/>
+    </row>
+    <row r="25" spans="2:5">
       <c r="B25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="17">
+      <c r="C25" s="18">
         <v>4</v>
       </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="19"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D25" s="19"/>
+      <c r="E25" s="20"/>
+    </row>
+    <row r="26" spans="2:5">
       <c r="B26" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="19"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D26" s="19"/>
+      <c r="E26" s="20"/>
+    </row>
+    <row r="27" spans="2:5">
       <c r="B27" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="13"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="24"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="26"/>
+    </row>
+    <row r="28" spans="2:5">
       <c r="B28" s="1" t="s">
         <v>27</v>
       </c>
@@ -1911,7 +1909,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B29" s="3">
         <v>1</v>
       </c>
@@ -1921,11 +1919,11 @@
       <c r="D29" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="E29" s="21" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="30" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B30" s="3">
         <v>2</v>
       </c>
@@ -1937,7 +1935,7 @@
       </c>
       <c r="E30" s="22"/>
     </row>
-    <row r="31" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B31" s="3">
         <v>3</v>
       </c>
@@ -1947,43 +1945,43 @@
       <c r="D31" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="21"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="14"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="16"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="23"/>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="B32" s="12"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="14"/>
+    </row>
+    <row r="34" spans="2:5">
       <c r="B34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="17">
+      <c r="C34" s="18">
         <v>5</v>
       </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="19"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="19"/>
+      <c r="E34" s="20"/>
+    </row>
+    <row r="35" spans="2:5">
       <c r="B35" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="18"/>
-      <c r="E35" s="19"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="19"/>
+      <c r="E35" s="20"/>
+    </row>
+    <row r="36" spans="2:5">
       <c r="B36" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="13"/>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C36" s="24"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="26"/>
+    </row>
+    <row r="37" spans="2:5">
       <c r="B37" s="1" t="s">
         <v>27</v>
       </c>
@@ -1997,7 +1995,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B38" s="3">
         <v>1</v>
       </c>
@@ -2011,41 +2009,41 @@
         <v>266</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="14"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="16"/>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5">
+      <c r="B39" s="12"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="14"/>
+    </row>
+    <row r="41" spans="2:5">
       <c r="B41" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C41" s="17">
+      <c r="C41" s="18">
         <v>6</v>
       </c>
-      <c r="D41" s="18"/>
-      <c r="E41" s="19"/>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D41" s="19"/>
+      <c r="E41" s="20"/>
+    </row>
+    <row r="42" spans="2:5">
       <c r="B42" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="17" t="s">
+      <c r="C42" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D42" s="18"/>
-      <c r="E42" s="19"/>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D42" s="19"/>
+      <c r="E42" s="20"/>
+    </row>
+    <row r="43" spans="2:5">
       <c r="B43" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="11"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="13"/>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C43" s="24"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="26"/>
+    </row>
+    <row r="44" spans="2:5">
       <c r="B44" s="1" t="s">
         <v>27</v>
       </c>
@@ -2059,7 +2057,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B45" s="3">
         <v>1</v>
       </c>
@@ -2069,11 +2067,11 @@
       <c r="D45" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E45" s="20" t="s">
+      <c r="E45" s="21" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="46" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B46" s="3">
         <v>2</v>
       </c>
@@ -2083,43 +2081,43 @@
       <c r="D46" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E46" s="21"/>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="14"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="16"/>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E46" s="23"/>
+    </row>
+    <row r="47" spans="2:5">
+      <c r="B47" s="12"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="14"/>
+    </row>
+    <row r="49" spans="2:5">
       <c r="B49" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="17">
+      <c r="C49" s="18">
         <v>7</v>
       </c>
-      <c r="D49" s="18"/>
-      <c r="E49" s="19"/>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D49" s="19"/>
+      <c r="E49" s="20"/>
+    </row>
+    <row r="50" spans="2:5">
       <c r="B50" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C50" s="17" t="s">
+      <c r="C50" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D50" s="18"/>
-      <c r="E50" s="19"/>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D50" s="19"/>
+      <c r="E50" s="20"/>
+    </row>
+    <row r="51" spans="2:5">
       <c r="B51" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C51" s="11"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="13"/>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C51" s="24"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="26"/>
+    </row>
+    <row r="52" spans="2:5">
       <c r="B52" s="1" t="s">
         <v>27</v>
       </c>
@@ -2133,7 +2131,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B53" s="3">
         <v>1</v>
       </c>
@@ -2147,41 +2145,41 @@
         <v>268</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="14"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="16"/>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:5">
+      <c r="B54" s="12"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="14"/>
+    </row>
+    <row r="56" spans="2:5">
       <c r="B56" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C56" s="17">
+      <c r="C56" s="18">
         <v>8</v>
       </c>
-      <c r="D56" s="18"/>
-      <c r="E56" s="19"/>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D56" s="19"/>
+      <c r="E56" s="20"/>
+    </row>
+    <row r="57" spans="2:5">
       <c r="B57" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C57" s="17" t="s">
+      <c r="C57" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D57" s="18"/>
-      <c r="E57" s="19"/>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D57" s="19"/>
+      <c r="E57" s="20"/>
+    </row>
+    <row r="58" spans="2:5">
       <c r="B58" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C58" s="11"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="13"/>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C58" s="24"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="26"/>
+    </row>
+    <row r="59" spans="2:5">
       <c r="B59" s="1" t="s">
         <v>27</v>
       </c>
@@ -2195,7 +2193,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B60" s="3">
         <v>1</v>
       </c>
@@ -2205,11 +2203,11 @@
       <c r="D60" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E60" s="20" t="s">
+      <c r="E60" s="21" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="61" spans="2:5" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:5" s="5" customFormat="1" ht="38.25">
       <c r="B61" s="3">
         <v>2</v>
       </c>
@@ -2221,7 +2219,7 @@
       </c>
       <c r="E61" s="22"/>
     </row>
-    <row r="62" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B62" s="3">
         <v>3</v>
       </c>
@@ -2231,43 +2229,43 @@
       <c r="D62" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E62" s="21"/>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="14"/>
-      <c r="C63" s="15"/>
-      <c r="D63" s="15"/>
-      <c r="E63" s="16"/>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E62" s="23"/>
+    </row>
+    <row r="63" spans="2:5">
+      <c r="B63" s="12"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="14"/>
+    </row>
+    <row r="65" spans="2:5">
       <c r="B65" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C65" s="17">
+      <c r="C65" s="18">
         <v>9</v>
       </c>
-      <c r="D65" s="18"/>
-      <c r="E65" s="19"/>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D65" s="19"/>
+      <c r="E65" s="20"/>
+    </row>
+    <row r="66" spans="2:5">
       <c r="B66" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C66" s="17" t="s">
+      <c r="C66" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D66" s="18"/>
-      <c r="E66" s="19"/>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D66" s="19"/>
+      <c r="E66" s="20"/>
+    </row>
+    <row r="67" spans="2:5">
       <c r="B67" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C67" s="11"/>
-      <c r="D67" s="12"/>
-      <c r="E67" s="13"/>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C67" s="24"/>
+      <c r="D67" s="25"/>
+      <c r="E67" s="26"/>
+    </row>
+    <row r="68" spans="2:5">
       <c r="B68" s="1" t="s">
         <v>27</v>
       </c>
@@ -2281,7 +2279,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B69" s="3">
         <v>1</v>
       </c>
@@ -2291,11 +2289,11 @@
       <c r="D69" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E69" s="20" t="s">
+      <c r="E69" s="21" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="70" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B70" s="3">
         <v>2</v>
       </c>
@@ -2307,7 +2305,7 @@
       </c>
       <c r="E70" s="22"/>
     </row>
-    <row r="71" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:5" s="5" customFormat="1">
       <c r="B71" s="3">
         <v>3</v>
       </c>
@@ -2317,43 +2315,43 @@
       <c r="D71" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="E71" s="21"/>
-    </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B72" s="14"/>
-      <c r="C72" s="15"/>
-      <c r="D72" s="15"/>
-      <c r="E72" s="16"/>
-    </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E71" s="23"/>
+    </row>
+    <row r="72" spans="2:5">
+      <c r="B72" s="12"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="14"/>
+    </row>
+    <row r="74" spans="2:5">
       <c r="B74" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C74" s="17">
+      <c r="C74" s="18">
         <v>10</v>
       </c>
-      <c r="D74" s="18"/>
-      <c r="E74" s="19"/>
-    </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D74" s="19"/>
+      <c r="E74" s="20"/>
+    </row>
+    <row r="75" spans="2:5">
       <c r="B75" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C75" s="17" t="s">
+      <c r="C75" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D75" s="18"/>
-      <c r="E75" s="19"/>
-    </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D75" s="19"/>
+      <c r="E75" s="20"/>
+    </row>
+    <row r="76" spans="2:5">
       <c r="B76" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C76" s="11"/>
-      <c r="D76" s="12"/>
-      <c r="E76" s="13"/>
-    </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C76" s="24"/>
+      <c r="D76" s="25"/>
+      <c r="E76" s="26"/>
+    </row>
+    <row r="77" spans="2:5">
       <c r="B77" s="1" t="s">
         <v>27</v>
       </c>
@@ -2367,7 +2365,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="78" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B78" s="3">
         <v>1</v>
       </c>
@@ -2377,11 +2375,11 @@
       <c r="D78" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E78" s="20" t="s">
+      <c r="E78" s="21" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="79" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B79" s="3">
         <v>2</v>
       </c>
@@ -2391,45 +2389,45 @@
       <c r="D79" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E79" s="21"/>
-    </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B80" s="14"/>
-      <c r="C80" s="15"/>
-      <c r="D80" s="15"/>
-      <c r="E80" s="16"/>
-    </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E79" s="23"/>
+    </row>
+    <row r="80" spans="2:5">
+      <c r="B80" s="12"/>
+      <c r="C80" s="13"/>
+      <c r="D80" s="13"/>
+      <c r="E80" s="14"/>
+    </row>
+    <row r="82" spans="2:5">
       <c r="B82" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C82" s="17">
+      <c r="C82" s="18">
         <v>11</v>
       </c>
-      <c r="D82" s="18"/>
-      <c r="E82" s="19"/>
-    </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D82" s="19"/>
+      <c r="E82" s="20"/>
+    </row>
+    <row r="83" spans="2:5">
       <c r="B83" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C83" s="17" t="s">
+      <c r="C83" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D83" s="18"/>
-      <c r="E83" s="19"/>
-    </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D83" s="19"/>
+      <c r="E83" s="20"/>
+    </row>
+    <row r="84" spans="2:5">
       <c r="B84" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C84" s="23" t="s">
+      <c r="C84" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D84" s="24"/>
-      <c r="E84" s="25"/>
-    </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D84" s="16"/>
+      <c r="E84" s="17"/>
+    </row>
+    <row r="85" spans="2:5">
       <c r="B85" s="1" t="s">
         <v>27</v>
       </c>
@@ -2443,7 +2441,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="86" spans="2:5" s="5" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:5" s="5" customFormat="1" ht="63.75">
       <c r="B86" s="3"/>
       <c r="C86" s="7" t="s">
         <v>54</v>
@@ -2455,43 +2453,43 @@
         <v>270</v>
       </c>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B87" s="14"/>
-      <c r="C87" s="15"/>
-      <c r="D87" s="15"/>
-      <c r="E87" s="16"/>
-    </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:5">
+      <c r="B87" s="12"/>
+      <c r="C87" s="13"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="14"/>
+    </row>
+    <row r="89" spans="2:5">
       <c r="B89" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C89" s="17">
+      <c r="C89" s="18">
         <v>12</v>
       </c>
-      <c r="D89" s="18"/>
-      <c r="E89" s="19"/>
-    </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D89" s="19"/>
+      <c r="E89" s="20"/>
+    </row>
+    <row r="90" spans="2:5">
       <c r="B90" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C90" s="17" t="s">
+      <c r="C90" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D90" s="18"/>
-      <c r="E90" s="19"/>
-    </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D90" s="19"/>
+      <c r="E90" s="20"/>
+    </row>
+    <row r="91" spans="2:5">
       <c r="B91" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C91" s="23" t="s">
+      <c r="C91" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D91" s="24"/>
-      <c r="E91" s="25"/>
-    </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D91" s="16"/>
+      <c r="E91" s="17"/>
+    </row>
+    <row r="92" spans="2:5">
       <c r="B92" s="1" t="s">
         <v>27</v>
       </c>
@@ -2505,7 +2503,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="93" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B93" s="3">
         <v>1</v>
       </c>
@@ -2519,43 +2517,43 @@
         <v>271</v>
       </c>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B94" s="14"/>
-      <c r="C94" s="15"/>
-      <c r="D94" s="15"/>
-      <c r="E94" s="16"/>
-    </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:5">
+      <c r="B94" s="12"/>
+      <c r="C94" s="13"/>
+      <c r="D94" s="13"/>
+      <c r="E94" s="14"/>
+    </row>
+    <row r="96" spans="2:5">
       <c r="B96" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C96" s="17">
+      <c r="C96" s="18">
         <v>13</v>
       </c>
-      <c r="D96" s="18"/>
-      <c r="E96" s="19"/>
-    </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D96" s="19"/>
+      <c r="E96" s="20"/>
+    </row>
+    <row r="97" spans="2:5">
       <c r="B97" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C97" s="17" t="s">
+      <c r="C97" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D97" s="18"/>
-      <c r="E97" s="19"/>
-    </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D97" s="19"/>
+      <c r="E97" s="20"/>
+    </row>
+    <row r="98" spans="2:5">
       <c r="B98" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C98" s="23" t="s">
+      <c r="C98" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D98" s="24"/>
-      <c r="E98" s="25"/>
-    </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D98" s="16"/>
+      <c r="E98" s="17"/>
+    </row>
+    <row r="99" spans="2:5">
       <c r="B99" s="1" t="s">
         <v>27</v>
       </c>
@@ -2569,7 +2567,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="100" spans="2:5" s="5" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:5" s="5" customFormat="1" ht="63.75">
       <c r="B100" s="3">
         <v>1</v>
       </c>
@@ -2579,11 +2577,11 @@
       <c r="D100" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E100" s="20" t="s">
+      <c r="E100" s="21" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="101" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B101" s="3">
         <v>2</v>
       </c>
@@ -2593,45 +2591,45 @@
       <c r="D101" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E101" s="21"/>
-    </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B102" s="14"/>
-      <c r="C102" s="15"/>
-      <c r="D102" s="15"/>
-      <c r="E102" s="16"/>
-    </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E101" s="23"/>
+    </row>
+    <row r="102" spans="2:5">
+      <c r="B102" s="12"/>
+      <c r="C102" s="13"/>
+      <c r="D102" s="13"/>
+      <c r="E102" s="14"/>
+    </row>
+    <row r="104" spans="2:5">
       <c r="B104" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C104" s="17">
+      <c r="C104" s="18">
         <v>14</v>
       </c>
-      <c r="D104" s="18"/>
-      <c r="E104" s="19"/>
-    </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D104" s="19"/>
+      <c r="E104" s="20"/>
+    </row>
+    <row r="105" spans="2:5">
       <c r="B105" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C105" s="17" t="s">
+      <c r="C105" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D105" s="18"/>
-      <c r="E105" s="19"/>
-    </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D105" s="19"/>
+      <c r="E105" s="20"/>
+    </row>
+    <row r="106" spans="2:5">
       <c r="B106" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C106" s="23" t="s">
+      <c r="C106" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D106" s="24"/>
-      <c r="E106" s="25"/>
-    </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D106" s="16"/>
+      <c r="E106" s="17"/>
+    </row>
+    <row r="107" spans="2:5">
       <c r="B107" s="1" t="s">
         <v>27</v>
       </c>
@@ -2645,7 +2643,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="108" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B108" s="3">
         <v>1</v>
       </c>
@@ -2655,11 +2653,11 @@
       <c r="D108" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E108" s="20" t="s">
+      <c r="E108" s="21" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="109" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B109" s="3">
         <v>2</v>
       </c>
@@ -2669,45 +2667,45 @@
       <c r="D109" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E109" s="21"/>
-    </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B110" s="14"/>
-      <c r="C110" s="15"/>
-      <c r="D110" s="15"/>
-      <c r="E110" s="16"/>
-    </row>
-    <row r="112" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E109" s="23"/>
+    </row>
+    <row r="110" spans="2:5">
+      <c r="B110" s="12"/>
+      <c r="C110" s="13"/>
+      <c r="D110" s="13"/>
+      <c r="E110" s="14"/>
+    </row>
+    <row r="112" spans="2:5">
       <c r="B112" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C112" s="17">
+      <c r="C112" s="18">
         <v>15</v>
       </c>
-      <c r="D112" s="18"/>
-      <c r="E112" s="19"/>
-    </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D112" s="19"/>
+      <c r="E112" s="20"/>
+    </row>
+    <row r="113" spans="2:5">
       <c r="B113" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C113" s="17" t="s">
+      <c r="C113" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D113" s="18"/>
-      <c r="E113" s="19"/>
-    </row>
-    <row r="114" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D113" s="19"/>
+      <c r="E113" s="20"/>
+    </row>
+    <row r="114" spans="2:5" ht="30.75" customHeight="1">
       <c r="B114" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C114" s="23" t="s">
+      <c r="C114" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="D114" s="24"/>
-      <c r="E114" s="25"/>
-    </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D114" s="16"/>
+      <c r="E114" s="17"/>
+    </row>
+    <row r="115" spans="2:5">
       <c r="B115" s="1" t="s">
         <v>27</v>
       </c>
@@ -2721,7 +2719,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="116" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B116" s="3">
         <v>1</v>
       </c>
@@ -2731,11 +2729,11 @@
       <c r="D116" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E116" s="20" t="s">
+      <c r="E116" s="21" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="117" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B117" s="3">
         <v>2</v>
       </c>
@@ -2747,7 +2745,7 @@
       </c>
       <c r="E117" s="22"/>
     </row>
-    <row r="118" spans="2:5" s="5" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:5" s="5" customFormat="1" ht="63.75">
       <c r="B118" s="3">
         <v>3</v>
       </c>
@@ -2757,45 +2755,45 @@
       <c r="D118" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E118" s="21"/>
-    </row>
-    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B119" s="14"/>
-      <c r="C119" s="15"/>
-      <c r="D119" s="15"/>
-      <c r="E119" s="16"/>
-    </row>
-    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E118" s="23"/>
+    </row>
+    <row r="119" spans="2:5">
+      <c r="B119" s="12"/>
+      <c r="C119" s="13"/>
+      <c r="D119" s="13"/>
+      <c r="E119" s="14"/>
+    </row>
+    <row r="121" spans="2:5">
       <c r="B121" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C121" s="17">
+      <c r="C121" s="18">
         <v>16</v>
       </c>
-      <c r="D121" s="18"/>
-      <c r="E121" s="19"/>
-    </row>
-    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D121" s="19"/>
+      <c r="E121" s="20"/>
+    </row>
+    <row r="122" spans="2:5">
       <c r="B122" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C122" s="17" t="s">
+      <c r="C122" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D122" s="18"/>
-      <c r="E122" s="19"/>
-    </row>
-    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D122" s="19"/>
+      <c r="E122" s="20"/>
+    </row>
+    <row r="123" spans="2:5">
       <c r="B123" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C123" s="23" t="s">
+      <c r="C123" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D123" s="24"/>
-      <c r="E123" s="25"/>
-    </row>
-    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D123" s="16"/>
+      <c r="E123" s="17"/>
+    </row>
+    <row r="124" spans="2:5">
       <c r="B124" s="1" t="s">
         <v>27</v>
       </c>
@@ -2809,7 +2807,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="125" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B125" s="3">
         <v>1</v>
       </c>
@@ -2819,11 +2817,11 @@
       <c r="D125" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E125" s="20" t="s">
+      <c r="E125" s="21" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="126" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B126" s="3">
         <v>2</v>
       </c>
@@ -2833,45 +2831,45 @@
       <c r="D126" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E126" s="21"/>
-    </row>
-    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B127" s="14"/>
-      <c r="C127" s="15"/>
-      <c r="D127" s="15"/>
-      <c r="E127" s="16"/>
-    </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E126" s="23"/>
+    </row>
+    <row r="127" spans="2:5">
+      <c r="B127" s="12"/>
+      <c r="C127" s="13"/>
+      <c r="D127" s="13"/>
+      <c r="E127" s="14"/>
+    </row>
+    <row r="129" spans="2:5">
       <c r="B129" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C129" s="17">
+      <c r="C129" s="18">
         <v>17</v>
       </c>
-      <c r="D129" s="18"/>
-      <c r="E129" s="19"/>
-    </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D129" s="19"/>
+      <c r="E129" s="20"/>
+    </row>
+    <row r="130" spans="2:5">
       <c r="B130" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C130" s="17" t="s">
+      <c r="C130" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D130" s="18"/>
-      <c r="E130" s="19"/>
-    </row>
-    <row r="131" spans="2:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D130" s="19"/>
+      <c r="E130" s="20"/>
+    </row>
+    <row r="131" spans="2:5" ht="27" customHeight="1">
       <c r="B131" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C131" s="23" t="s">
+      <c r="C131" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D131" s="24"/>
-      <c r="E131" s="25"/>
-    </row>
-    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D131" s="16"/>
+      <c r="E131" s="17"/>
+    </row>
+    <row r="132" spans="2:5">
       <c r="B132" s="1" t="s">
         <v>27</v>
       </c>
@@ -2885,7 +2883,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="133" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B133" s="3">
         <v>1</v>
       </c>
@@ -2895,11 +2893,11 @@
       <c r="D133" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E133" s="20" t="s">
+      <c r="E133" s="21" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="134" spans="2:5" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:5" s="5" customFormat="1" ht="38.25">
       <c r="B134" s="3">
         <v>2</v>
       </c>
@@ -2909,45 +2907,45 @@
       <c r="D134" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E134" s="21"/>
-    </row>
-    <row r="135" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B135" s="14"/>
-      <c r="C135" s="15"/>
-      <c r="D135" s="15"/>
-      <c r="E135" s="16"/>
-    </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E134" s="23"/>
+    </row>
+    <row r="135" spans="2:5">
+      <c r="B135" s="12"/>
+      <c r="C135" s="13"/>
+      <c r="D135" s="13"/>
+      <c r="E135" s="14"/>
+    </row>
+    <row r="137" spans="2:5">
       <c r="B137" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C137" s="17">
+      <c r="C137" s="18">
         <v>18</v>
       </c>
-      <c r="D137" s="18"/>
-      <c r="E137" s="19"/>
-    </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D137" s="19"/>
+      <c r="E137" s="20"/>
+    </row>
+    <row r="138" spans="2:5">
       <c r="B138" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C138" s="17" t="s">
+      <c r="C138" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D138" s="18"/>
-      <c r="E138" s="19"/>
-    </row>
-    <row r="139" spans="2:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D138" s="19"/>
+      <c r="E138" s="20"/>
+    </row>
+    <row r="139" spans="2:5" ht="25.5" customHeight="1">
       <c r="B139" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C139" s="23" t="s">
+      <c r="C139" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D139" s="24"/>
-      <c r="E139" s="25"/>
-    </row>
-    <row r="140" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D139" s="16"/>
+      <c r="E139" s="17"/>
+    </row>
+    <row r="140" spans="2:5">
       <c r="B140" s="1" t="s">
         <v>27</v>
       </c>
@@ -2961,7 +2959,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="141" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B141" s="3">
         <v>1</v>
       </c>
@@ -2975,43 +2973,43 @@
         <v>276</v>
       </c>
     </row>
-    <row r="142" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B142" s="14"/>
-      <c r="C142" s="15"/>
-      <c r="D142" s="15"/>
-      <c r="E142" s="16"/>
-    </row>
-    <row r="144" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:5">
+      <c r="B142" s="12"/>
+      <c r="C142" s="13"/>
+      <c r="D142" s="13"/>
+      <c r="E142" s="14"/>
+    </row>
+    <row r="144" spans="2:5">
       <c r="B144" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C144" s="17">
+      <c r="C144" s="18">
         <v>19</v>
       </c>
-      <c r="D144" s="18"/>
-      <c r="E144" s="19"/>
-    </row>
-    <row r="145" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D144" s="19"/>
+      <c r="E144" s="20"/>
+    </row>
+    <row r="145" spans="2:5">
       <c r="B145" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C145" s="17" t="s">
+      <c r="C145" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D145" s="18"/>
-      <c r="E145" s="19"/>
-    </row>
-    <row r="146" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D145" s="19"/>
+      <c r="E145" s="20"/>
+    </row>
+    <row r="146" spans="2:5">
       <c r="B146" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C146" s="23" t="s">
+      <c r="C146" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D146" s="24"/>
-      <c r="E146" s="25"/>
-    </row>
-    <row r="147" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D146" s="16"/>
+      <c r="E146" s="17"/>
+    </row>
+    <row r="147" spans="2:5">
       <c r="B147" s="1" t="s">
         <v>27</v>
       </c>
@@ -3025,7 +3023,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="148" spans="2:5" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:5" ht="76.5">
       <c r="B148" s="3">
         <v>1</v>
       </c>
@@ -3035,11 +3033,11 @@
       <c r="D148" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E148" s="20" t="s">
+      <c r="E148" s="21" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="149" spans="2:5" ht="51" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:5" ht="51">
       <c r="B149" s="3">
         <v>2</v>
       </c>
@@ -3051,7 +3049,7 @@
       </c>
       <c r="E149" s="22"/>
     </row>
-    <row r="150" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B150" s="3">
         <v>3</v>
       </c>
@@ -3063,7 +3061,7 @@
       </c>
       <c r="E150" s="22"/>
     </row>
-    <row r="151" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B151" s="3">
         <v>4</v>
       </c>
@@ -3073,45 +3071,45 @@
       <c r="D151" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E151" s="21"/>
-    </row>
-    <row r="152" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B152" s="14"/>
-      <c r="C152" s="15"/>
-      <c r="D152" s="15"/>
-      <c r="E152" s="16"/>
-    </row>
-    <row r="154" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E151" s="23"/>
+    </row>
+    <row r="152" spans="2:5">
+      <c r="B152" s="12"/>
+      <c r="C152" s="13"/>
+      <c r="D152" s="13"/>
+      <c r="E152" s="14"/>
+    </row>
+    <row r="154" spans="2:5">
       <c r="B154" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C154" s="17">
+      <c r="C154" s="18">
         <v>20</v>
       </c>
-      <c r="D154" s="18"/>
-      <c r="E154" s="19"/>
-    </row>
-    <row r="155" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D154" s="19"/>
+      <c r="E154" s="20"/>
+    </row>
+    <row r="155" spans="2:5">
       <c r="B155" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C155" s="17" t="s">
+      <c r="C155" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D155" s="18"/>
-      <c r="E155" s="19"/>
-    </row>
-    <row r="156" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D155" s="19"/>
+      <c r="E155" s="20"/>
+    </row>
+    <row r="156" spans="2:5" ht="27.75" customHeight="1">
       <c r="B156" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C156" s="23" t="s">
+      <c r="C156" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D156" s="24"/>
-      <c r="E156" s="25"/>
-    </row>
-    <row r="157" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D156" s="16"/>
+      <c r="E156" s="17"/>
+    </row>
+    <row r="157" spans="2:5">
       <c r="B157" s="1" t="s">
         <v>27</v>
       </c>
@@ -3125,7 +3123,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="158" spans="2:5" s="5" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:5" s="5" customFormat="1" ht="76.5">
       <c r="B158" s="3">
         <v>1</v>
       </c>
@@ -3139,43 +3137,43 @@
         <v>278</v>
       </c>
     </row>
-    <row r="159" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B159" s="14"/>
-      <c r="C159" s="15"/>
-      <c r="D159" s="15"/>
-      <c r="E159" s="16"/>
-    </row>
-    <row r="161" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:5">
+      <c r="B159" s="12"/>
+      <c r="C159" s="13"/>
+      <c r="D159" s="13"/>
+      <c r="E159" s="14"/>
+    </row>
+    <row r="161" spans="2:5">
       <c r="B161" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C161" s="17">
+      <c r="C161" s="18">
         <v>21</v>
       </c>
-      <c r="D161" s="18"/>
-      <c r="E161" s="19"/>
-    </row>
-    <row r="162" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D161" s="19"/>
+      <c r="E161" s="20"/>
+    </row>
+    <row r="162" spans="2:5">
       <c r="B162" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C162" s="17" t="s">
+      <c r="C162" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D162" s="18"/>
-      <c r="E162" s="19"/>
-    </row>
-    <row r="163" spans="2:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D162" s="19"/>
+      <c r="E162" s="20"/>
+    </row>
+    <row r="163" spans="2:5" ht="42.75" customHeight="1">
       <c r="B163" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C163" s="23" t="s">
+      <c r="C163" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="D163" s="24"/>
-      <c r="E163" s="25"/>
-    </row>
-    <row r="164" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D163" s="16"/>
+      <c r="E163" s="17"/>
+    </row>
+    <row r="164" spans="2:5">
       <c r="B164" s="1" t="s">
         <v>27</v>
       </c>
@@ -3189,7 +3187,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="165" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B165" s="3"/>
       <c r="C165" s="7" t="s">
         <v>86</v>
@@ -3197,11 +3195,11 @@
       <c r="D165" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E165" s="20" t="s">
+      <c r="E165" s="21" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="166" spans="2:5" ht="51" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:5" ht="51">
       <c r="B166" s="3"/>
       <c r="C166" s="7" t="s">
         <v>89</v>
@@ -3211,7 +3209,7 @@
       </c>
       <c r="E166" s="22"/>
     </row>
-    <row r="167" spans="2:5" ht="51" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:5" ht="51">
       <c r="B167" s="3"/>
       <c r="C167" s="7" t="s">
         <v>90</v>
@@ -3219,45 +3217,45 @@
       <c r="D167" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="E167" s="21"/>
-    </row>
-    <row r="168" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B168" s="14"/>
-      <c r="C168" s="15"/>
-      <c r="D168" s="15"/>
-      <c r="E168" s="16"/>
-    </row>
-    <row r="170" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E167" s="23"/>
+    </row>
+    <row r="168" spans="2:5">
+      <c r="B168" s="12"/>
+      <c r="C168" s="13"/>
+      <c r="D168" s="13"/>
+      <c r="E168" s="14"/>
+    </row>
+    <row r="170" spans="2:5">
       <c r="B170" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C170" s="17">
+      <c r="C170" s="18">
         <v>22</v>
       </c>
-      <c r="D170" s="18"/>
-      <c r="E170" s="19"/>
-    </row>
-    <row r="171" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D170" s="19"/>
+      <c r="E170" s="20"/>
+    </row>
+    <row r="171" spans="2:5">
       <c r="B171" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C171" s="17" t="s">
+      <c r="C171" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D171" s="18"/>
-      <c r="E171" s="19"/>
-    </row>
-    <row r="172" spans="2:5" s="5" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D171" s="19"/>
+      <c r="E171" s="20"/>
+    </row>
+    <row r="172" spans="2:5" s="5" customFormat="1" ht="30.75" customHeight="1">
       <c r="B172" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C172" s="23" t="s">
+      <c r="C172" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D172" s="24"/>
-      <c r="E172" s="25"/>
-    </row>
-    <row r="173" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D172" s="16"/>
+      <c r="E172" s="17"/>
+    </row>
+    <row r="173" spans="2:5">
       <c r="B173" s="1" t="s">
         <v>27</v>
       </c>
@@ -3271,7 +3269,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="174" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:5" ht="38.25">
       <c r="B174" s="3">
         <v>1</v>
       </c>
@@ -3281,11 +3279,11 @@
       <c r="D174" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E174" s="20" t="s">
+      <c r="E174" s="21" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="175" spans="2:5" ht="51" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:5" ht="51">
       <c r="B175" s="3">
         <v>2</v>
       </c>
@@ -3297,7 +3295,7 @@
       </c>
       <c r="E175" s="22"/>
     </row>
-    <row r="176" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:5" ht="38.25">
       <c r="B176" s="3">
         <v>3</v>
       </c>
@@ -3309,7 +3307,7 @@
       </c>
       <c r="E176" s="22"/>
     </row>
-    <row r="177" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:5" ht="25.5">
       <c r="B177" s="3">
         <v>4</v>
       </c>
@@ -3321,7 +3319,7 @@
       </c>
       <c r="E177" s="22"/>
     </row>
-    <row r="178" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:5" ht="25.5">
       <c r="B178" s="3">
         <v>5</v>
       </c>
@@ -3331,45 +3329,45 @@
       <c r="D178" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E178" s="21"/>
-    </row>
-    <row r="179" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B179" s="14"/>
-      <c r="C179" s="15"/>
-      <c r="D179" s="15"/>
-      <c r="E179" s="16"/>
-    </row>
-    <row r="181" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E178" s="23"/>
+    </row>
+    <row r="179" spans="2:5" s="5" customFormat="1">
+      <c r="B179" s="12"/>
+      <c r="C179" s="13"/>
+      <c r="D179" s="13"/>
+      <c r="E179" s="14"/>
+    </row>
+    <row r="181" spans="2:5">
       <c r="B181" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C181" s="17">
+      <c r="C181" s="18">
         <v>23</v>
       </c>
-      <c r="D181" s="18"/>
-      <c r="E181" s="19"/>
-    </row>
-    <row r="182" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D181" s="19"/>
+      <c r="E181" s="20"/>
+    </row>
+    <row r="182" spans="2:5">
       <c r="B182" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C182" s="17" t="s">
+      <c r="C182" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D182" s="18"/>
-      <c r="E182" s="19"/>
-    </row>
-    <row r="183" spans="2:5" s="5" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D182" s="19"/>
+      <c r="E182" s="20"/>
+    </row>
+    <row r="183" spans="2:5" s="5" customFormat="1" ht="30.75" customHeight="1">
       <c r="B183" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C183" s="23" t="s">
+      <c r="C183" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D183" s="24"/>
-      <c r="E183" s="25"/>
-    </row>
-    <row r="184" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D183" s="16"/>
+      <c r="E183" s="17"/>
+    </row>
+    <row r="184" spans="2:5">
       <c r="B184" s="1" t="s">
         <v>27</v>
       </c>
@@ -3383,7 +3381,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="185" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:5" ht="38.25">
       <c r="B185" s="3">
         <v>1</v>
       </c>
@@ -3397,49 +3395,49 @@
         <v>281</v>
       </c>
     </row>
-    <row r="186" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B186" s="14"/>
-      <c r="C186" s="15"/>
-      <c r="D186" s="15"/>
-      <c r="E186" s="16"/>
-    </row>
-    <row r="187" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:5" s="5" customFormat="1">
+      <c r="B186" s="12"/>
+      <c r="C186" s="13"/>
+      <c r="D186" s="13"/>
+      <c r="E186" s="14"/>
+    </row>
+    <row r="187" spans="2:5">
       <c r="B187" s="2"/>
       <c r="C187" s="2"/>
       <c r="D187" s="2"/>
       <c r="E187" s="9"/>
     </row>
-    <row r="188" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:5">
       <c r="B188" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C188" s="17">
+      <c r="C188" s="18">
         <v>24</v>
       </c>
-      <c r="D188" s="18"/>
-      <c r="E188" s="19"/>
-    </row>
-    <row r="189" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D188" s="19"/>
+      <c r="E188" s="20"/>
+    </row>
+    <row r="189" spans="2:5">
       <c r="B189" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C189" s="17" t="s">
+      <c r="C189" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D189" s="18"/>
-      <c r="E189" s="19"/>
-    </row>
-    <row r="190" spans="2:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D189" s="19"/>
+      <c r="E189" s="20"/>
+    </row>
+    <row r="190" spans="2:5" ht="27" customHeight="1">
       <c r="B190" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C190" s="23" t="s">
+      <c r="C190" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D190" s="24"/>
-      <c r="E190" s="25"/>
-    </row>
-    <row r="191" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D190" s="16"/>
+      <c r="E190" s="17"/>
+    </row>
+    <row r="191" spans="2:5">
       <c r="B191" s="1" t="s">
         <v>27</v>
       </c>
@@ -3453,7 +3451,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="192" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:5" ht="38.25">
       <c r="B192" s="3">
         <v>1</v>
       </c>
@@ -3467,43 +3465,43 @@
         <v>282</v>
       </c>
     </row>
-    <row r="193" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B193" s="14"/>
-      <c r="C193" s="15"/>
-      <c r="D193" s="15"/>
-      <c r="E193" s="16"/>
-    </row>
-    <row r="195" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:5" s="5" customFormat="1">
+      <c r="B193" s="12"/>
+      <c r="C193" s="13"/>
+      <c r="D193" s="13"/>
+      <c r="E193" s="14"/>
+    </row>
+    <row r="195" spans="2:5">
       <c r="B195" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C195" s="17">
+      <c r="C195" s="18">
         <v>25</v>
       </c>
-      <c r="D195" s="18"/>
-      <c r="E195" s="19"/>
-    </row>
-    <row r="196" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D195" s="19"/>
+      <c r="E195" s="20"/>
+    </row>
+    <row r="196" spans="2:5">
       <c r="B196" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C196" s="17" t="s">
+      <c r="C196" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D196" s="18"/>
-      <c r="E196" s="19"/>
-    </row>
-    <row r="197" spans="2:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D196" s="19"/>
+      <c r="E196" s="20"/>
+    </row>
+    <row r="197" spans="2:5" ht="25.5" customHeight="1">
       <c r="B197" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C197" s="23" t="s">
+      <c r="C197" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D197" s="24"/>
-      <c r="E197" s="25"/>
-    </row>
-    <row r="198" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D197" s="16"/>
+      <c r="E197" s="17"/>
+    </row>
+    <row r="198" spans="2:5">
       <c r="B198" s="1" t="s">
         <v>27</v>
       </c>
@@ -3517,7 +3515,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="199" spans="2:5" ht="51" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:5" ht="51">
       <c r="B199" s="3">
         <v>1</v>
       </c>
@@ -3531,43 +3529,43 @@
         <v>283</v>
       </c>
     </row>
-    <row r="200" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B200" s="14"/>
-      <c r="C200" s="15"/>
-      <c r="D200" s="15"/>
-      <c r="E200" s="16"/>
-    </row>
-    <row r="202" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:5" s="5" customFormat="1">
+      <c r="B200" s="12"/>
+      <c r="C200" s="13"/>
+      <c r="D200" s="13"/>
+      <c r="E200" s="14"/>
+    </row>
+    <row r="202" spans="2:5">
       <c r="B202" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C202" s="17">
+      <c r="C202" s="18">
         <v>26</v>
       </c>
-      <c r="D202" s="18"/>
-      <c r="E202" s="19"/>
-    </row>
-    <row r="203" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D202" s="19"/>
+      <c r="E202" s="20"/>
+    </row>
+    <row r="203" spans="2:5">
       <c r="B203" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C203" s="17" t="s">
+      <c r="C203" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D203" s="18"/>
-      <c r="E203" s="19"/>
-    </row>
-    <row r="204" spans="2:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D203" s="19"/>
+      <c r="E203" s="20"/>
+    </row>
+    <row r="204" spans="2:5" ht="27" customHeight="1">
       <c r="B204" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C204" s="23" t="s">
+      <c r="C204" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="D204" s="24"/>
-      <c r="E204" s="25"/>
-    </row>
-    <row r="205" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D204" s="16"/>
+      <c r="E204" s="17"/>
+    </row>
+    <row r="205" spans="2:5">
       <c r="B205" s="1" t="s">
         <v>27</v>
       </c>
@@ -3581,7 +3579,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="206" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:5" ht="25.5">
       <c r="B206" s="3">
         <v>1</v>
       </c>
@@ -3591,11 +3589,11 @@
       <c r="D206" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="E206" s="20" t="s">
+      <c r="E206" s="21" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="207" spans="2:5" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:5" ht="89.25">
       <c r="B207" s="3">
         <v>2</v>
       </c>
@@ -3607,7 +3605,7 @@
       </c>
       <c r="E207" s="22"/>
     </row>
-    <row r="208" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:5" ht="25.5">
       <c r="B208" s="3">
         <v>3</v>
       </c>
@@ -3617,45 +3615,45 @@
       <c r="D208" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E208" s="21"/>
-    </row>
-    <row r="209" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B209" s="14"/>
-      <c r="C209" s="15"/>
-      <c r="D209" s="15"/>
-      <c r="E209" s="16"/>
-    </row>
-    <row r="211" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E208" s="23"/>
+    </row>
+    <row r="209" spans="2:5" s="5" customFormat="1">
+      <c r="B209" s="12"/>
+      <c r="C209" s="13"/>
+      <c r="D209" s="13"/>
+      <c r="E209" s="14"/>
+    </row>
+    <row r="211" spans="2:5">
       <c r="B211" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C211" s="17">
+      <c r="C211" s="18">
         <v>27</v>
       </c>
-      <c r="D211" s="18"/>
-      <c r="E211" s="19"/>
-    </row>
-    <row r="212" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D211" s="19"/>
+      <c r="E211" s="20"/>
+    </row>
+    <row r="212" spans="2:5">
       <c r="B212" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C212" s="17" t="s">
+      <c r="C212" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="D212" s="18"/>
-      <c r="E212" s="19"/>
-    </row>
-    <row r="213" spans="2:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D212" s="19"/>
+      <c r="E212" s="20"/>
+    </row>
+    <row r="213" spans="2:5" ht="27" customHeight="1">
       <c r="B213" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C213" s="23" t="s">
+      <c r="C213" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="D213" s="24"/>
-      <c r="E213" s="25"/>
-    </row>
-    <row r="214" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D213" s="16"/>
+      <c r="E213" s="17"/>
+    </row>
+    <row r="214" spans="2:5">
       <c r="B214" s="1" t="s">
         <v>27</v>
       </c>
@@ -3669,7 +3667,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="215" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:5" ht="38.25">
       <c r="B215" s="3">
         <v>1</v>
       </c>
@@ -3683,43 +3681,43 @@
         <v>285</v>
       </c>
     </row>
-    <row r="216" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B216" s="14"/>
-      <c r="C216" s="15"/>
-      <c r="D216" s="15"/>
-      <c r="E216" s="16"/>
-    </row>
-    <row r="218" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:5" s="5" customFormat="1">
+      <c r="B216" s="12"/>
+      <c r="C216" s="13"/>
+      <c r="D216" s="13"/>
+      <c r="E216" s="14"/>
+    </row>
+    <row r="218" spans="2:5">
       <c r="B218" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C218" s="17">
+      <c r="C218" s="18">
         <v>28</v>
       </c>
-      <c r="D218" s="18"/>
-      <c r="E218" s="19"/>
-    </row>
-    <row r="219" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D218" s="19"/>
+      <c r="E218" s="20"/>
+    </row>
+    <row r="219" spans="2:5">
       <c r="B219" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C219" s="17" t="s">
+      <c r="C219" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D219" s="18"/>
-      <c r="E219" s="19"/>
-    </row>
-    <row r="220" spans="2:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D219" s="19"/>
+      <c r="E219" s="20"/>
+    </row>
+    <row r="220" spans="2:5" ht="28.5" customHeight="1">
       <c r="B220" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C220" s="23" t="s">
+      <c r="C220" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="D220" s="24"/>
-      <c r="E220" s="25"/>
-    </row>
-    <row r="221" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D220" s="16"/>
+      <c r="E220" s="17"/>
+    </row>
+    <row r="221" spans="2:5">
       <c r="B221" s="1" t="s">
         <v>27</v>
       </c>
@@ -3733,7 +3731,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="222" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:5" ht="38.25">
       <c r="B222" s="3">
         <v>1</v>
       </c>
@@ -3747,43 +3745,43 @@
         <v>286</v>
       </c>
     </row>
-    <row r="223" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B223" s="14"/>
-      <c r="C223" s="15"/>
-      <c r="D223" s="15"/>
-      <c r="E223" s="16"/>
-    </row>
-    <row r="225" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:5" s="5" customFormat="1">
+      <c r="B223" s="12"/>
+      <c r="C223" s="13"/>
+      <c r="D223" s="13"/>
+      <c r="E223" s="14"/>
+    </row>
+    <row r="225" spans="2:5">
       <c r="B225" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C225" s="17">
+      <c r="C225" s="18">
         <v>29</v>
       </c>
-      <c r="D225" s="18"/>
-      <c r="E225" s="19"/>
-    </row>
-    <row r="226" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D225" s="19"/>
+      <c r="E225" s="20"/>
+    </row>
+    <row r="226" spans="2:5">
       <c r="B226" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C226" s="17" t="s">
+      <c r="C226" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D226" s="18"/>
-      <c r="E226" s="19"/>
-    </row>
-    <row r="227" spans="2:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D226" s="19"/>
+      <c r="E226" s="20"/>
+    </row>
+    <row r="227" spans="2:5" ht="29.25" customHeight="1">
       <c r="B227" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C227" s="23" t="s">
+      <c r="C227" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="D227" s="24"/>
-      <c r="E227" s="25"/>
-    </row>
-    <row r="228" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D227" s="16"/>
+      <c r="E227" s="17"/>
+    </row>
+    <row r="228" spans="2:5">
       <c r="B228" s="1" t="s">
         <v>27</v>
       </c>
@@ -3797,7 +3795,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="229" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:5" ht="38.25">
       <c r="B229" s="3">
         <v>1</v>
       </c>
@@ -3811,43 +3809,43 @@
         <v>287</v>
       </c>
     </row>
-    <row r="230" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B230" s="14"/>
-      <c r="C230" s="15"/>
-      <c r="D230" s="15"/>
-      <c r="E230" s="16"/>
-    </row>
-    <row r="232" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:5" s="5" customFormat="1">
+      <c r="B230" s="12"/>
+      <c r="C230" s="13"/>
+      <c r="D230" s="13"/>
+      <c r="E230" s="14"/>
+    </row>
+    <row r="232" spans="2:5">
       <c r="B232" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C232" s="17">
+      <c r="C232" s="18">
         <v>30</v>
       </c>
-      <c r="D232" s="18"/>
-      <c r="E232" s="19"/>
-    </row>
-    <row r="233" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D232" s="19"/>
+      <c r="E232" s="20"/>
+    </row>
+    <row r="233" spans="2:5">
       <c r="B233" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C233" s="17" t="s">
+      <c r="C233" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="D233" s="18"/>
-      <c r="E233" s="19"/>
-    </row>
-    <row r="234" spans="2:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D233" s="19"/>
+      <c r="E233" s="20"/>
+    </row>
+    <row r="234" spans="2:5" ht="26.25" customHeight="1">
       <c r="B234" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C234" s="23" t="s">
+      <c r="C234" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="D234" s="24"/>
-      <c r="E234" s="25"/>
-    </row>
-    <row r="235" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D234" s="16"/>
+      <c r="E234" s="17"/>
+    </row>
+    <row r="235" spans="2:5">
       <c r="B235" s="1" t="s">
         <v>27</v>
       </c>
@@ -3861,7 +3859,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="236" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:5" ht="25.5">
       <c r="B236" s="3">
         <v>1</v>
       </c>
@@ -3871,11 +3869,11 @@
       <c r="D236" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="E236" s="20" t="s">
+      <c r="E236" s="21" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="237" spans="2:5" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:5" ht="89.25">
       <c r="B237" s="3">
         <v>2</v>
       </c>
@@ -3887,7 +3885,7 @@
       </c>
       <c r="E237" s="22"/>
     </row>
-    <row r="238" spans="2:5" ht="51" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:5" ht="51">
       <c r="B238" s="3">
         <v>3</v>
       </c>
@@ -3899,7 +3897,7 @@
       </c>
       <c r="E238" s="22"/>
     </row>
-    <row r="239" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:5" ht="38.25">
       <c r="B239" s="3">
         <v>4</v>
       </c>
@@ -3911,7 +3909,7 @@
       </c>
       <c r="E239" s="22"/>
     </row>
-    <row r="240" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:5" ht="25.5">
       <c r="B240" s="3">
         <v>5</v>
       </c>
@@ -3921,45 +3919,45 @@
       <c r="D240" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E240" s="21"/>
-    </row>
-    <row r="241" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B241" s="14"/>
-      <c r="C241" s="15"/>
-      <c r="D241" s="15"/>
-      <c r="E241" s="16"/>
-    </row>
-    <row r="243" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E240" s="23"/>
+    </row>
+    <row r="241" spans="2:5" s="5" customFormat="1">
+      <c r="B241" s="12"/>
+      <c r="C241" s="13"/>
+      <c r="D241" s="13"/>
+      <c r="E241" s="14"/>
+    </row>
+    <row r="243" spans="2:5">
       <c r="B243" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C243" s="17">
+      <c r="C243" s="18">
         <v>31</v>
       </c>
-      <c r="D243" s="18"/>
-      <c r="E243" s="19"/>
-    </row>
-    <row r="244" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D243" s="19"/>
+      <c r="E243" s="20"/>
+    </row>
+    <row r="244" spans="2:5">
       <c r="B244" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C244" s="17" t="s">
+      <c r="C244" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="D244" s="18"/>
-      <c r="E244" s="19"/>
-    </row>
-    <row r="245" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D244" s="19"/>
+      <c r="E244" s="20"/>
+    </row>
+    <row r="245" spans="2:5" ht="30" customHeight="1">
       <c r="B245" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C245" s="23" t="s">
+      <c r="C245" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="D245" s="24"/>
-      <c r="E245" s="25"/>
-    </row>
-    <row r="246" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D245" s="16"/>
+      <c r="E245" s="17"/>
+    </row>
+    <row r="246" spans="2:5">
       <c r="B246" s="1" t="s">
         <v>27</v>
       </c>
@@ -3973,7 +3971,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="247" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:5" ht="25.5">
       <c r="B247" s="3">
         <v>1</v>
       </c>
@@ -3983,11 +3981,11 @@
       <c r="D247" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="E247" s="20" t="s">
+      <c r="E247" s="21" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="248" spans="2:5" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:5" ht="89.25">
       <c r="B248" s="3">
         <v>2</v>
       </c>
@@ -3999,7 +3997,7 @@
       </c>
       <c r="E248" s="22"/>
     </row>
-    <row r="249" spans="2:5" ht="51" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:5" ht="51">
       <c r="B249" s="3">
         <v>3</v>
       </c>
@@ -4011,7 +4009,7 @@
       </c>
       <c r="E249" s="22"/>
     </row>
-    <row r="250" spans="2:5" ht="51" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:5" ht="51">
       <c r="B250" s="3">
         <v>4</v>
       </c>
@@ -4021,45 +4019,45 @@
       <c r="D250" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="E250" s="21"/>
-    </row>
-    <row r="251" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B251" s="14"/>
-      <c r="C251" s="15"/>
-      <c r="D251" s="15"/>
-      <c r="E251" s="16"/>
-    </row>
-    <row r="253" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E250" s="23"/>
+    </row>
+    <row r="251" spans="2:5" s="5" customFormat="1">
+      <c r="B251" s="12"/>
+      <c r="C251" s="13"/>
+      <c r="D251" s="13"/>
+      <c r="E251" s="14"/>
+    </row>
+    <row r="253" spans="2:5">
       <c r="B253" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C253" s="17">
+      <c r="C253" s="18">
         <v>32</v>
       </c>
-      <c r="D253" s="18"/>
-      <c r="E253" s="19"/>
-    </row>
-    <row r="254" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D253" s="19"/>
+      <c r="E253" s="20"/>
+    </row>
+    <row r="254" spans="2:5">
       <c r="B254" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C254" s="17" t="s">
+      <c r="C254" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D254" s="18"/>
-      <c r="E254" s="19"/>
-    </row>
-    <row r="255" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D254" s="19"/>
+      <c r="E254" s="20"/>
+    </row>
+    <row r="255" spans="2:5" ht="30" customHeight="1">
       <c r="B255" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C255" s="23" t="s">
+      <c r="C255" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="D255" s="24"/>
-      <c r="E255" s="25"/>
-    </row>
-    <row r="256" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D255" s="16"/>
+      <c r="E255" s="17"/>
+    </row>
+    <row r="256" spans="2:5">
       <c r="B256" s="1" t="s">
         <v>27</v>
       </c>
@@ -4073,7 +4071,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="257" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:5" ht="25.5">
       <c r="B257" s="3">
         <v>1</v>
       </c>
@@ -4083,11 +4081,11 @@
       <c r="D257" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="E257" s="20" t="s">
+      <c r="E257" s="21" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="258" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B258" s="3">
         <v>2</v>
       </c>
@@ -4099,7 +4097,7 @@
       </c>
       <c r="E258" s="22"/>
     </row>
-    <row r="259" spans="2:5" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:5" s="5" customFormat="1" ht="38.25">
       <c r="B259" s="3">
         <v>3</v>
       </c>
@@ -4109,45 +4107,45 @@
       <c r="D259" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="E259" s="21"/>
-    </row>
-    <row r="260" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B260" s="14"/>
-      <c r="C260" s="15"/>
-      <c r="D260" s="15"/>
-      <c r="E260" s="16"/>
-    </row>
-    <row r="262" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E259" s="23"/>
+    </row>
+    <row r="260" spans="2:5">
+      <c r="B260" s="12"/>
+      <c r="C260" s="13"/>
+      <c r="D260" s="13"/>
+      <c r="E260" s="14"/>
+    </row>
+    <row r="262" spans="2:5">
       <c r="B262" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C262" s="17">
+      <c r="C262" s="18">
         <v>33</v>
       </c>
-      <c r="D262" s="18"/>
-      <c r="E262" s="19"/>
-    </row>
-    <row r="263" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D262" s="19"/>
+      <c r="E262" s="20"/>
+    </row>
+    <row r="263" spans="2:5">
       <c r="B263" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C263" s="17" t="s">
+      <c r="C263" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="D263" s="18"/>
-      <c r="E263" s="19"/>
-    </row>
-    <row r="264" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D263" s="19"/>
+      <c r="E263" s="20"/>
+    </row>
+    <row r="264" spans="2:5" ht="30" customHeight="1">
       <c r="B264" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C264" s="23" t="s">
+      <c r="C264" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="D264" s="24"/>
-      <c r="E264" s="25"/>
-    </row>
-    <row r="265" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D264" s="16"/>
+      <c r="E264" s="17"/>
+    </row>
+    <row r="265" spans="2:5">
       <c r="B265" s="1" t="s">
         <v>27</v>
       </c>
@@ -4161,7 +4159,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="266" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B266" s="3">
         <v>1</v>
       </c>
@@ -4175,7 +4173,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="267" spans="2:5" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:5" s="5" customFormat="1" ht="38.25">
       <c r="B267" s="3">
         <v>2</v>
       </c>
@@ -4185,45 +4183,45 @@
       <c r="D267" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="E267" s="21"/>
-    </row>
-    <row r="268" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B268" s="14"/>
-      <c r="C268" s="15"/>
-      <c r="D268" s="15"/>
-      <c r="E268" s="16"/>
-    </row>
-    <row r="270" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E267" s="23"/>
+    </row>
+    <row r="268" spans="2:5">
+      <c r="B268" s="12"/>
+      <c r="C268" s="13"/>
+      <c r="D268" s="13"/>
+      <c r="E268" s="14"/>
+    </row>
+    <row r="270" spans="2:5">
       <c r="B270" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C270" s="17">
+      <c r="C270" s="18">
         <v>34</v>
       </c>
-      <c r="D270" s="18"/>
-      <c r="E270" s="19"/>
-    </row>
-    <row r="271" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D270" s="19"/>
+      <c r="E270" s="20"/>
+    </row>
+    <row r="271" spans="2:5">
       <c r="B271" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C271" s="17" t="s">
+      <c r="C271" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D271" s="18"/>
-      <c r="E271" s="19"/>
-    </row>
-    <row r="272" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D271" s="19"/>
+      <c r="E271" s="20"/>
+    </row>
+    <row r="272" spans="2:5" ht="27.75" customHeight="1">
       <c r="B272" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C272" s="23" t="s">
+      <c r="C272" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D272" s="24"/>
-      <c r="E272" s="25"/>
-    </row>
-    <row r="273" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D272" s="16"/>
+      <c r="E272" s="17"/>
+    </row>
+    <row r="273" spans="2:5">
       <c r="B273" s="1" t="s">
         <v>27</v>
       </c>
@@ -4237,7 +4235,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="274" spans="2:5" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="274" spans="2:5" s="5" customFormat="1" ht="38.25">
       <c r="B274" s="3">
         <v>1</v>
       </c>
@@ -4251,43 +4249,43 @@
         <v>292</v>
       </c>
     </row>
-    <row r="275" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B275" s="14"/>
-      <c r="C275" s="15"/>
-      <c r="D275" s="15"/>
-      <c r="E275" s="16"/>
-    </row>
-    <row r="277" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="2:5">
+      <c r="B275" s="12"/>
+      <c r="C275" s="13"/>
+      <c r="D275" s="13"/>
+      <c r="E275" s="14"/>
+    </row>
+    <row r="277" spans="2:5">
       <c r="B277" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C277" s="17">
+      <c r="C277" s="18">
         <v>35</v>
       </c>
-      <c r="D277" s="18"/>
-      <c r="E277" s="19"/>
-    </row>
-    <row r="278" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D277" s="19"/>
+      <c r="E277" s="20"/>
+    </row>
+    <row r="278" spans="2:5">
       <c r="B278" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C278" s="17" t="s">
+      <c r="C278" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D278" s="18"/>
-      <c r="E278" s="19"/>
-    </row>
-    <row r="279" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D278" s="19"/>
+      <c r="E278" s="20"/>
+    </row>
+    <row r="279" spans="2:5" ht="33" customHeight="1">
       <c r="B279" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C279" s="23" t="s">
+      <c r="C279" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="D279" s="24"/>
-      <c r="E279" s="25"/>
-    </row>
-    <row r="280" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D279" s="16"/>
+      <c r="E279" s="17"/>
+    </row>
+    <row r="280" spans="2:5">
       <c r="B280" s="1" t="s">
         <v>27</v>
       </c>
@@ -4301,7 +4299,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="281" spans="2:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="281" spans="2:5" s="5" customFormat="1" ht="25.5">
       <c r="B281" s="3">
         <v>1</v>
       </c>
@@ -4315,43 +4313,43 @@
         <v>293</v>
       </c>
     </row>
-    <row r="282" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B282" s="14"/>
-      <c r="C282" s="15"/>
-      <c r="D282" s="15"/>
-      <c r="E282" s="16"/>
-    </row>
-    <row r="284" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="2:5">
+      <c r="B282" s="12"/>
+      <c r="C282" s="13"/>
+      <c r="D282" s="13"/>
+      <c r="E282" s="14"/>
+    </row>
+    <row r="284" spans="2:5">
       <c r="B284" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C284" s="17">
+      <c r="C284" s="18">
         <v>36</v>
       </c>
-      <c r="D284" s="18"/>
-      <c r="E284" s="19"/>
-    </row>
-    <row r="285" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D284" s="19"/>
+      <c r="E284" s="20"/>
+    </row>
+    <row r="285" spans="2:5">
       <c r="B285" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C285" s="17" t="s">
+      <c r="C285" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D285" s="18"/>
-      <c r="E285" s="19"/>
-    </row>
-    <row r="286" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D285" s="19"/>
+      <c r="E285" s="20"/>
+    </row>
+    <row r="286" spans="2:5" ht="30.75" customHeight="1">
       <c r="B286" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C286" s="23" t="s">
+      <c r="C286" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D286" s="24"/>
-      <c r="E286" s="25"/>
-    </row>
-    <row r="287" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D286" s="16"/>
+      <c r="E286" s="17"/>
+    </row>
+    <row r="287" spans="2:5">
       <c r="B287" s="1" t="s">
         <v>27</v>
       </c>
@@ -4365,7 +4363,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="288" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="288" spans="2:5" ht="38.25">
       <c r="B288" s="3">
         <v>1</v>
       </c>
@@ -4379,43 +4377,43 @@
         <v>294</v>
       </c>
     </row>
-    <row r="289" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B289" s="14"/>
-      <c r="C289" s="15"/>
-      <c r="D289" s="15"/>
-      <c r="E289" s="16"/>
-    </row>
-    <row r="291" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="2:5">
+      <c r="B289" s="12"/>
+      <c r="C289" s="13"/>
+      <c r="D289" s="13"/>
+      <c r="E289" s="14"/>
+    </row>
+    <row r="291" spans="2:5">
       <c r="B291" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C291" s="17">
+      <c r="C291" s="18">
         <v>37</v>
       </c>
-      <c r="D291" s="18"/>
-      <c r="E291" s="19"/>
-    </row>
-    <row r="292" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D291" s="19"/>
+      <c r="E291" s="20"/>
+    </row>
+    <row r="292" spans="2:5">
       <c r="B292" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C292" s="17" t="s">
+      <c r="C292" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="D292" s="18"/>
-      <c r="E292" s="19"/>
-    </row>
-    <row r="293" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D292" s="19"/>
+      <c r="E292" s="20"/>
+    </row>
+    <row r="293" spans="2:5">
       <c r="B293" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C293" s="23" t="s">
+      <c r="C293" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D293" s="24"/>
-      <c r="E293" s="25"/>
-    </row>
-    <row r="294" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D293" s="16"/>
+      <c r="E293" s="17"/>
+    </row>
+    <row r="294" spans="2:5">
       <c r="B294" s="1" t="s">
         <v>27</v>
       </c>
@@ -4429,7 +4427,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="295" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="295" spans="2:5" ht="38.25">
       <c r="B295" s="3">
         <v>1</v>
       </c>
@@ -4443,43 +4441,43 @@
         <v>296</v>
       </c>
     </row>
-    <row r="296" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B296" s="14"/>
-      <c r="C296" s="15"/>
-      <c r="D296" s="15"/>
-      <c r="E296" s="16"/>
-    </row>
-    <row r="298" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="2:5">
+      <c r="B296" s="12"/>
+      <c r="C296" s="13"/>
+      <c r="D296" s="13"/>
+      <c r="E296" s="14"/>
+    </row>
+    <row r="298" spans="2:5">
       <c r="B298" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C298" s="17">
+      <c r="C298" s="18">
         <v>38</v>
       </c>
-      <c r="D298" s="18"/>
-      <c r="E298" s="19"/>
-    </row>
-    <row r="299" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D298" s="19"/>
+      <c r="E298" s="20"/>
+    </row>
+    <row r="299" spans="2:5">
       <c r="B299" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C299" s="17" t="s">
+      <c r="C299" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="D299" s="18"/>
-      <c r="E299" s="19"/>
-    </row>
-    <row r="300" spans="2:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D299" s="19"/>
+      <c r="E299" s="20"/>
+    </row>
+    <row r="300" spans="2:5" ht="27" customHeight="1">
       <c r="B300" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C300" s="23" t="s">
+      <c r="C300" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="D300" s="24"/>
-      <c r="E300" s="25"/>
-    </row>
-    <row r="301" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D300" s="16"/>
+      <c r="E300" s="17"/>
+    </row>
+    <row r="301" spans="2:5">
       <c r="B301" s="1" t="s">
         <v>27</v>
       </c>
@@ -4493,7 +4491,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="302" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="302" spans="2:5" ht="38.25">
       <c r="B302" s="3">
         <v>1</v>
       </c>
@@ -4507,75 +4505,99 @@
         <v>295</v>
       </c>
     </row>
-    <row r="303" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B303" s="14"/>
-      <c r="C303" s="15"/>
-      <c r="D303" s="15"/>
-      <c r="E303" s="16"/>
+    <row r="303" spans="2:5">
+      <c r="B303" s="12"/>
+      <c r="C303" s="13"/>
+      <c r="D303" s="13"/>
+      <c r="E303" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="172">
-    <mergeCell ref="B303:E303"/>
-    <mergeCell ref="C300:E300"/>
-    <mergeCell ref="C299:E299"/>
-    <mergeCell ref="C298:E298"/>
-    <mergeCell ref="B296:E296"/>
-    <mergeCell ref="C293:E293"/>
-    <mergeCell ref="C292:E292"/>
-    <mergeCell ref="C291:E291"/>
-    <mergeCell ref="C279:E279"/>
-    <mergeCell ref="B282:E282"/>
-    <mergeCell ref="C284:E284"/>
-    <mergeCell ref="C285:E285"/>
-    <mergeCell ref="C286:E286"/>
-    <mergeCell ref="B289:E289"/>
-    <mergeCell ref="C232:E232"/>
-    <mergeCell ref="C233:E233"/>
-    <mergeCell ref="C234:E234"/>
-    <mergeCell ref="B241:E241"/>
-    <mergeCell ref="E236:E240"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C226:E226"/>
-    <mergeCell ref="C197:E197"/>
-    <mergeCell ref="B200:E200"/>
-    <mergeCell ref="C202:E202"/>
-    <mergeCell ref="C203:E203"/>
-    <mergeCell ref="C204:E204"/>
-    <mergeCell ref="B209:E209"/>
-    <mergeCell ref="C227:E227"/>
-    <mergeCell ref="B230:E230"/>
-    <mergeCell ref="C218:E218"/>
-    <mergeCell ref="C219:E219"/>
-    <mergeCell ref="C220:E220"/>
-    <mergeCell ref="B223:E223"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="E60:E62"/>
-    <mergeCell ref="C188:E188"/>
-    <mergeCell ref="C189:E189"/>
-    <mergeCell ref="C190:E190"/>
-    <mergeCell ref="B193:E193"/>
-    <mergeCell ref="C195:E195"/>
-    <mergeCell ref="C196:E196"/>
-    <mergeCell ref="C183:E183"/>
-    <mergeCell ref="B186:E186"/>
-    <mergeCell ref="C211:E211"/>
-    <mergeCell ref="C212:E212"/>
-    <mergeCell ref="C213:E213"/>
-    <mergeCell ref="B216:E216"/>
-    <mergeCell ref="E206:E208"/>
-    <mergeCell ref="C104:E104"/>
-    <mergeCell ref="C105:E105"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="B110:E110"/>
-    <mergeCell ref="C181:E181"/>
-    <mergeCell ref="C182:E182"/>
-    <mergeCell ref="E108:E109"/>
-    <mergeCell ref="E116:E118"/>
-    <mergeCell ref="E125:E126"/>
-    <mergeCell ref="E133:E134"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C76:E76"/>
+    <mergeCell ref="B80:E80"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="E78:E79"/>
+    <mergeCell ref="E69:E71"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="B63:E63"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="B72:E72"/>
+    <mergeCell ref="C98:E98"/>
+    <mergeCell ref="B102:E102"/>
+    <mergeCell ref="E100:E101"/>
+    <mergeCell ref="C82:E82"/>
+    <mergeCell ref="C83:E83"/>
+    <mergeCell ref="C84:E84"/>
+    <mergeCell ref="B87:E87"/>
+    <mergeCell ref="C96:E96"/>
+    <mergeCell ref="C97:E97"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C90:E90"/>
+    <mergeCell ref="C91:E91"/>
+    <mergeCell ref="B94:E94"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="B127:E127"/>
+    <mergeCell ref="C129:E129"/>
+    <mergeCell ref="C130:E130"/>
+    <mergeCell ref="C131:E131"/>
+    <mergeCell ref="B135:E135"/>
+    <mergeCell ref="C112:E112"/>
+    <mergeCell ref="C113:E113"/>
+    <mergeCell ref="C114:E114"/>
+    <mergeCell ref="B119:E119"/>
+    <mergeCell ref="C121:E121"/>
+    <mergeCell ref="C122:E122"/>
+    <mergeCell ref="C144:E144"/>
+    <mergeCell ref="C145:E145"/>
+    <mergeCell ref="C146:E146"/>
+    <mergeCell ref="B152:E152"/>
+    <mergeCell ref="E148:E151"/>
+    <mergeCell ref="C137:E137"/>
+    <mergeCell ref="C138:E138"/>
+    <mergeCell ref="C139:E139"/>
+    <mergeCell ref="B142:E142"/>
+    <mergeCell ref="B179:E179"/>
+    <mergeCell ref="E165:E167"/>
+    <mergeCell ref="E174:E178"/>
+    <mergeCell ref="C154:E154"/>
+    <mergeCell ref="C155:E155"/>
+    <mergeCell ref="C156:E156"/>
+    <mergeCell ref="B159:E159"/>
+    <mergeCell ref="C161:E161"/>
+    <mergeCell ref="C162:E162"/>
     <mergeCell ref="C278:E278"/>
     <mergeCell ref="C245:E245"/>
     <mergeCell ref="B251:E251"/>
@@ -4597,110 +4619,86 @@
     <mergeCell ref="C272:E272"/>
     <mergeCell ref="B275:E275"/>
     <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C195:E195"/>
+    <mergeCell ref="C196:E196"/>
+    <mergeCell ref="C183:E183"/>
+    <mergeCell ref="B186:E186"/>
+    <mergeCell ref="C211:E211"/>
+    <mergeCell ref="C212:E212"/>
+    <mergeCell ref="C213:E213"/>
+    <mergeCell ref="B216:E216"/>
+    <mergeCell ref="E206:E208"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="E60:E62"/>
+    <mergeCell ref="C188:E188"/>
+    <mergeCell ref="C189:E189"/>
+    <mergeCell ref="C190:E190"/>
+    <mergeCell ref="B193:E193"/>
+    <mergeCell ref="C104:E104"/>
+    <mergeCell ref="C105:E105"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="B110:E110"/>
+    <mergeCell ref="C181:E181"/>
+    <mergeCell ref="C182:E182"/>
+    <mergeCell ref="E108:E109"/>
+    <mergeCell ref="E116:E118"/>
+    <mergeCell ref="E125:E126"/>
+    <mergeCell ref="E133:E134"/>
     <mergeCell ref="C163:E163"/>
     <mergeCell ref="B168:E168"/>
     <mergeCell ref="C170:E170"/>
     <mergeCell ref="C171:E171"/>
     <mergeCell ref="C172:E172"/>
-    <mergeCell ref="B179:E179"/>
-    <mergeCell ref="E165:E167"/>
-    <mergeCell ref="E174:E178"/>
-    <mergeCell ref="C154:E154"/>
-    <mergeCell ref="C155:E155"/>
-    <mergeCell ref="C156:E156"/>
-    <mergeCell ref="B159:E159"/>
-    <mergeCell ref="C161:E161"/>
-    <mergeCell ref="C162:E162"/>
-    <mergeCell ref="C144:E144"/>
-    <mergeCell ref="C145:E145"/>
-    <mergeCell ref="C146:E146"/>
-    <mergeCell ref="B152:E152"/>
-    <mergeCell ref="E148:E151"/>
-    <mergeCell ref="C137:E137"/>
-    <mergeCell ref="C138:E138"/>
-    <mergeCell ref="C139:E139"/>
-    <mergeCell ref="B142:E142"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="B127:E127"/>
-    <mergeCell ref="C129:E129"/>
-    <mergeCell ref="C130:E130"/>
-    <mergeCell ref="C131:E131"/>
-    <mergeCell ref="B135:E135"/>
-    <mergeCell ref="C112:E112"/>
-    <mergeCell ref="C113:E113"/>
-    <mergeCell ref="C114:E114"/>
-    <mergeCell ref="B119:E119"/>
-    <mergeCell ref="C121:E121"/>
-    <mergeCell ref="C122:E122"/>
-    <mergeCell ref="C98:E98"/>
-    <mergeCell ref="B102:E102"/>
-    <mergeCell ref="E100:E101"/>
-    <mergeCell ref="C82:E82"/>
-    <mergeCell ref="C83:E83"/>
-    <mergeCell ref="C84:E84"/>
-    <mergeCell ref="B87:E87"/>
-    <mergeCell ref="C96:E96"/>
-    <mergeCell ref="C97:E97"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C90:E90"/>
-    <mergeCell ref="C91:E91"/>
-    <mergeCell ref="B94:E94"/>
-    <mergeCell ref="C76:E76"/>
-    <mergeCell ref="B80:E80"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="E78:E79"/>
-    <mergeCell ref="E69:E71"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="B63:E63"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="B72:E72"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C232:E232"/>
+    <mergeCell ref="C233:E233"/>
+    <mergeCell ref="C234:E234"/>
+    <mergeCell ref="B241:E241"/>
+    <mergeCell ref="E236:E240"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C226:E226"/>
+    <mergeCell ref="C197:E197"/>
+    <mergeCell ref="B200:E200"/>
+    <mergeCell ref="C202:E202"/>
+    <mergeCell ref="C203:E203"/>
+    <mergeCell ref="C204:E204"/>
+    <mergeCell ref="B209:E209"/>
+    <mergeCell ref="C227:E227"/>
+    <mergeCell ref="B230:E230"/>
+    <mergeCell ref="C218:E218"/>
+    <mergeCell ref="C219:E219"/>
+    <mergeCell ref="C220:E220"/>
+    <mergeCell ref="B223:E223"/>
+    <mergeCell ref="B303:E303"/>
+    <mergeCell ref="C300:E300"/>
+    <mergeCell ref="C299:E299"/>
+    <mergeCell ref="C298:E298"/>
+    <mergeCell ref="B296:E296"/>
+    <mergeCell ref="C293:E293"/>
+    <mergeCell ref="C292:E292"/>
+    <mergeCell ref="C291:E291"/>
+    <mergeCell ref="C279:E279"/>
+    <mergeCell ref="B282:E282"/>
+    <mergeCell ref="C284:E284"/>
+    <mergeCell ref="C285:E285"/>
+    <mergeCell ref="C286:E286"/>
+    <mergeCell ref="B289:E289"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="2.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.5703125" style="2"/>
     <col min="2" max="2" width="4.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -4710,7 +4708,7 @@
     <col min="6" max="16384" width="2.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5">
       <c r="B2" s="1" t="s">
         <v>32</v>
       </c>
@@ -4724,7 +4722,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5">
       <c r="B3" s="3" t="s">
         <v>262</v>
       </c>
@@ -4734,9 +4732,9 @@
       <c r="D3" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E3" s="26"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="2:5">
       <c r="B4" s="3" t="s">
         <v>263</v>
       </c>
@@ -4746,9 +4744,9 @@
       <c r="D4" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="26"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="2:5">
       <c r="B5" s="3" t="s">
         <v>264</v>
       </c>
@@ -4758,9 +4756,9 @@
       <c r="D5" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E5" s="26"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" spans="2:5">
       <c r="B6" s="3" t="s">
         <v>265</v>
       </c>
@@ -4770,9 +4768,9 @@
       <c r="D6" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E6" s="26"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="2:5">
       <c r="B7" s="3" t="s">
         <v>266</v>
       </c>
@@ -4782,9 +4780,9 @@
       <c r="D7" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E7" s="26"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="2:5">
       <c r="B8" s="3" t="s">
         <v>267</v>
       </c>
@@ -4794,9 +4792,9 @@
       <c r="D8" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E8" s="26"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="2:5">
       <c r="B9" s="3" t="s">
         <v>268</v>
       </c>
@@ -4806,9 +4804,9 @@
       <c r="D9" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E9" s="26"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="2:5">
       <c r="B10" s="3" t="s">
         <v>173</v>
       </c>
@@ -4818,9 +4816,9 @@
       <c r="D10" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="E10" s="26"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="2:5">
       <c r="B11" s="3" t="s">
         <v>174</v>
       </c>
@@ -4830,9 +4828,9 @@
       <c r="D11" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="E11" s="26"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="2:5">
       <c r="B12" s="3" t="s">
         <v>175</v>
       </c>
@@ -4842,9 +4840,9 @@
       <c r="D12" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="E12" s="26"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="2:5">
       <c r="B13" s="3" t="s">
         <v>176</v>
       </c>
@@ -4854,9 +4852,9 @@
       <c r="D13" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="E13" s="26"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14" spans="2:5">
       <c r="B14" s="3" t="s">
         <v>177</v>
       </c>
@@ -4866,9 +4864,9 @@
       <c r="D14" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="E14" s="26"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="11"/>
+    </row>
+    <row r="15" spans="2:5">
       <c r="B15" s="3" t="s">
         <v>178</v>
       </c>
@@ -4878,9 +4876,9 @@
       <c r="D15" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="E15" s="26"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="11"/>
+    </row>
+    <row r="16" spans="2:5">
       <c r="B16" s="3" t="s">
         <v>179</v>
       </c>
@@ -4890,9 +4888,9 @@
       <c r="D16" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="E16" s="26"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="11"/>
+    </row>
+    <row r="17" spans="2:5">
       <c r="B17" s="3" t="s">
         <v>180</v>
       </c>
@@ -4902,9 +4900,9 @@
       <c r="D17" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="E17" s="26"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="11"/>
+    </row>
+    <row r="18" spans="2:5">
       <c r="B18" s="3" t="s">
         <v>181</v>
       </c>
@@ -4914,9 +4912,9 @@
       <c r="D18" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="E18" s="26"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="11"/>
+    </row>
+    <row r="19" spans="2:5">
       <c r="B19" s="3" t="s">
         <v>182</v>
       </c>
@@ -4926,9 +4924,9 @@
       <c r="D19" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="E19" s="26"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="11"/>
+    </row>
+    <row r="20" spans="2:5">
       <c r="B20" s="3" t="s">
         <v>183</v>
       </c>
@@ -4938,9 +4936,9 @@
       <c r="D20" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="E20" s="26"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="11"/>
+    </row>
+    <row r="21" spans="2:5">
       <c r="B21" s="3" t="s">
         <v>184</v>
       </c>
@@ -4950,9 +4948,9 @@
       <c r="D21" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="E21" s="26"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="11"/>
+    </row>
+    <row r="22" spans="2:5">
       <c r="B22" s="3" t="s">
         <v>185</v>
       </c>
@@ -4962,9 +4960,9 @@
       <c r="D22" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="E22" s="26"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="11"/>
+    </row>
+    <row r="23" spans="2:5">
       <c r="B23" s="3" t="s">
         <v>186</v>
       </c>
@@ -4974,9 +4972,9 @@
       <c r="D23" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="E23" s="26"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="11"/>
+    </row>
+    <row r="24" spans="2:5">
       <c r="B24" s="3" t="s">
         <v>187</v>
       </c>
@@ -4986,9 +4984,9 @@
       <c r="D24" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="E24" s="26"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="11"/>
+    </row>
+    <row r="25" spans="2:5">
       <c r="B25" s="3" t="s">
         <v>188</v>
       </c>
@@ -4998,9 +4996,9 @@
       <c r="D25" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="E25" s="26"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="11"/>
+    </row>
+    <row r="26" spans="2:5">
       <c r="B26" s="3" t="s">
         <v>189</v>
       </c>
@@ -5010,9 +5008,9 @@
       <c r="D26" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="E26" s="26"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="11"/>
+    </row>
+    <row r="27" spans="2:5">
       <c r="B27" s="3" t="s">
         <v>190</v>
       </c>
@@ -5022,9 +5020,9 @@
       <c r="D27" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="E27" s="26"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="11"/>
+    </row>
+    <row r="28" spans="2:5">
       <c r="B28" s="3" t="s">
         <v>200</v>
       </c>
@@ -5034,9 +5032,9 @@
       <c r="D28" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="E28" s="26"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="11"/>
+    </row>
+    <row r="29" spans="2:5">
       <c r="B29" s="3" t="s">
         <v>201</v>
       </c>
@@ -5046,9 +5044,9 @@
       <c r="D29" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="E29" s="26"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="11"/>
+    </row>
+    <row r="30" spans="2:5">
       <c r="B30" s="3" t="s">
         <v>202</v>
       </c>
@@ -5058,9 +5056,9 @@
       <c r="D30" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="E30" s="26"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="11"/>
+    </row>
+    <row r="31" spans="2:5">
       <c r="B31" s="3" t="s">
         <v>203</v>
       </c>
@@ -5070,9 +5068,9 @@
       <c r="D31" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="E31" s="26"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="11"/>
+    </row>
+    <row r="32" spans="2:5">
       <c r="B32" s="3" t="s">
         <v>207</v>
       </c>
@@ -5082,9 +5080,9 @@
       <c r="D32" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="E32" s="26"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="11"/>
+    </row>
+    <row r="33" spans="2:5">
       <c r="B33" s="3" t="s">
         <v>208</v>
       </c>
@@ -5094,9 +5092,9 @@
       <c r="D33" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="E33" s="26"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="11"/>
+    </row>
+    <row r="34" spans="2:5">
       <c r="B34" s="3" t="s">
         <v>209</v>
       </c>
@@ -5106,9 +5104,9 @@
       <c r="D34" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="E34" s="26"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="11"/>
+    </row>
+    <row r="35" spans="2:5">
       <c r="B35" s="3" t="s">
         <v>210</v>
       </c>
@@ -5118,9 +5116,9 @@
       <c r="D35" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="E35" s="26"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="11"/>
+    </row>
+    <row r="36" spans="2:5">
       <c r="B36" s="3" t="s">
         <v>211</v>
       </c>
@@ -5130,9 +5128,9 @@
       <c r="D36" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E36" s="26"/>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="11"/>
+    </row>
+    <row r="37" spans="2:5">
       <c r="B37" s="3" t="s">
         <v>212</v>
       </c>
@@ -5142,9 +5140,9 @@
       <c r="D37" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E37" s="26"/>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="11"/>
+    </row>
+    <row r="38" spans="2:5">
       <c r="B38" s="3" t="s">
         <v>269</v>
       </c>
@@ -5154,9 +5152,9 @@
       <c r="D38" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E38" s="26"/>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="11"/>
+    </row>
+    <row r="39" spans="2:5">
       <c r="B39" s="3" t="s">
         <v>270</v>
       </c>
@@ -5166,9 +5164,9 @@
       <c r="D39" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E39" s="26"/>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="11"/>
+    </row>
+    <row r="40" spans="2:5">
       <c r="B40" s="3" t="s">
         <v>271</v>
       </c>
@@ -5178,9 +5176,9 @@
       <c r="D40" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E40" s="26"/>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="11"/>
+    </row>
+    <row r="41" spans="2:5">
       <c r="B41" s="3" t="s">
         <v>272</v>
       </c>
@@ -5190,9 +5188,9 @@
       <c r="D41" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E41" s="26"/>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E41" s="11"/>
+    </row>
+    <row r="42" spans="2:5">
       <c r="B42" s="3" t="s">
         <v>273</v>
       </c>
@@ -5202,9 +5200,9 @@
       <c r="D42" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E42" s="26"/>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E42" s="11"/>
+    </row>
+    <row r="43" spans="2:5">
       <c r="B43" s="3" t="s">
         <v>225</v>
       </c>
@@ -5214,9 +5212,9 @@
       <c r="D43" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="E43" s="26"/>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E43" s="11"/>
+    </row>
+    <row r="44" spans="2:5">
       <c r="B44" s="3" t="s">
         <v>226</v>
       </c>
@@ -5226,9 +5224,9 @@
       <c r="D44" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="E44" s="26"/>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E44" s="11"/>
+    </row>
+    <row r="45" spans="2:5">
       <c r="B45" s="3" t="s">
         <v>227</v>
       </c>
@@ -5238,9 +5236,9 @@
       <c r="D45" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="E45" s="26"/>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E45" s="11"/>
+    </row>
+    <row r="46" spans="2:5">
       <c r="B46" s="3" t="s">
         <v>274</v>
       </c>
@@ -5250,9 +5248,9 @@
       <c r="D46" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E46" s="26"/>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E46" s="11"/>
+    </row>
+    <row r="47" spans="2:5">
       <c r="B47" s="3" t="s">
         <v>275</v>
       </c>
@@ -5262,9 +5260,9 @@
       <c r="D47" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E47" s="26"/>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E47" s="11"/>
+    </row>
+    <row r="48" spans="2:5">
       <c r="B48" s="3" t="s">
         <v>276</v>
       </c>
@@ -5274,9 +5272,9 @@
       <c r="D48" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E48" s="26"/>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E48" s="11"/>
+    </row>
+    <row r="49" spans="2:5">
       <c r="B49" s="3" t="s">
         <v>277</v>
       </c>
@@ -5286,9 +5284,9 @@
       <c r="D49" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E49" s="26"/>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E49" s="11"/>
+    </row>
+    <row r="50" spans="2:5">
       <c r="B50" s="3" t="s">
         <v>278</v>
       </c>
@@ -5298,9 +5296,9 @@
       <c r="D50" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E50" s="26"/>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E50" s="11"/>
+    </row>
+    <row r="51" spans="2:5">
       <c r="B51" s="3" t="s">
         <v>279</v>
       </c>
@@ -5310,9 +5308,9 @@
       <c r="D51" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E51" s="26"/>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E51" s="11"/>
+    </row>
+    <row r="52" spans="2:5">
       <c r="B52" s="3" t="s">
         <v>280</v>
       </c>
@@ -5322,9 +5320,9 @@
       <c r="D52" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E52" s="26"/>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E52" s="11"/>
+    </row>
+    <row r="53" spans="2:5">
       <c r="B53" s="3" t="s">
         <v>281</v>
       </c>
@@ -5334,9 +5332,9 @@
       <c r="D53" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E53" s="26"/>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E53" s="11"/>
+    </row>
+    <row r="54" spans="2:5">
       <c r="B54" s="3" t="s">
         <v>282</v>
       </c>
@@ -5346,9 +5344,9 @@
       <c r="D54" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E54" s="26"/>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E54" s="11"/>
+    </row>
+    <row r="55" spans="2:5">
       <c r="B55" s="3" t="s">
         <v>283</v>
       </c>
@@ -5358,9 +5356,9 @@
       <c r="D55" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E55" s="26"/>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E55" s="11"/>
+    </row>
+    <row r="56" spans="2:5">
       <c r="B56" s="3" t="s">
         <v>284</v>
       </c>
@@ -5370,9 +5368,9 @@
       <c r="D56" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E56" s="26"/>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E56" s="11"/>
+    </row>
+    <row r="57" spans="2:5">
       <c r="B57" s="3" t="s">
         <v>285</v>
       </c>
@@ -5382,9 +5380,9 @@
       <c r="D57" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E57" s="26"/>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E57" s="11"/>
+    </row>
+    <row r="58" spans="2:5">
       <c r="B58" s="3" t="s">
         <v>286</v>
       </c>
@@ -5394,9 +5392,9 @@
       <c r="D58" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E58" s="26"/>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E58" s="11"/>
+    </row>
+    <row r="59" spans="2:5">
       <c r="B59" s="3" t="s">
         <v>287</v>
       </c>
@@ -5406,9 +5404,9 @@
       <c r="D59" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E59" s="26"/>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E59" s="11"/>
+    </row>
+    <row r="60" spans="2:5">
       <c r="B60" s="3" t="s">
         <v>288</v>
       </c>
@@ -5418,9 +5416,9 @@
       <c r="D60" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E60" s="26"/>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E60" s="11"/>
+    </row>
+    <row r="61" spans="2:5">
       <c r="B61" s="3" t="s">
         <v>289</v>
       </c>
@@ -5430,9 +5428,9 @@
       <c r="D61" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E61" s="26"/>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E61" s="11"/>
+    </row>
+    <row r="62" spans="2:5">
       <c r="B62" s="3" t="s">
         <v>290</v>
       </c>
@@ -5442,9 +5440,9 @@
       <c r="D62" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E62" s="26"/>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E62" s="11"/>
+    </row>
+    <row r="63" spans="2:5">
       <c r="B63" s="3" t="s">
         <v>291</v>
       </c>
@@ -5454,9 +5452,9 @@
       <c r="D63" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E63" s="26"/>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E63" s="11"/>
+    </row>
+    <row r="64" spans="2:5">
       <c r="B64" s="3" t="s">
         <v>292</v>
       </c>
@@ -5466,9 +5464,9 @@
       <c r="D64" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E64" s="26"/>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E64" s="11"/>
+    </row>
+    <row r="65" spans="2:5">
       <c r="B65" s="3" t="s">
         <v>293</v>
       </c>
@@ -5478,9 +5476,9 @@
       <c r="D65" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E65" s="26"/>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E65" s="11"/>
+    </row>
+    <row r="66" spans="2:5">
       <c r="B66" s="3" t="s">
         <v>294</v>
       </c>
@@ -5490,9 +5488,9 @@
       <c r="D66" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E66" s="26"/>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E66" s="11"/>
+    </row>
+    <row r="67" spans="2:5">
       <c r="B67" s="3" t="s">
         <v>258</v>
       </c>
@@ -5502,9 +5500,9 @@
       <c r="D67" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="E67" s="26"/>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E67" s="11"/>
+    </row>
+    <row r="68" spans="2:5">
       <c r="B68" s="3" t="s">
         <v>259</v>
       </c>
@@ -5514,9 +5512,9 @@
       <c r="D68" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="E68" s="26"/>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E68" s="11"/>
+    </row>
+    <row r="69" spans="2:5">
       <c r="B69" s="3" t="s">
         <v>260</v>
       </c>
@@ -5526,9 +5524,9 @@
       <c r="D69" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="E69" s="26"/>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E69" s="11"/>
+    </row>
+    <row r="70" spans="2:5">
       <c r="B70" s="3" t="s">
         <v>261</v>
       </c>
@@ -5538,9 +5536,9 @@
       <c r="D70" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="E70" s="26"/>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E70" s="11"/>
+    </row>
+    <row r="71" spans="2:5">
       <c r="B71" s="3" t="s">
         <v>295</v>
       </c>
@@ -5550,7 +5548,7 @@
       <c r="D71" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E71" s="26"/>
+      <c r="E71" s="11"/>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>